<commit_message>
20250916 confused, so i commit for a restore point
</commit_message>
<xml_diff>
--- a/sweep_measurements.xlsx
+++ b/sweep_measurements.xlsx
@@ -703,10 +703,10 @@
     </row>
     <row r="2" ht="60" customHeight="1">
       <c r="A2" t="n">
-        <v>4.602265357971191</v>
+        <v>4.295692920684814</v>
       </c>
       <c r="B2" t="n">
-        <v>9.672922611236572</v>
+        <v>12.95009994506836</v>
       </c>
       <c r="C2" t="n">
         <v>2</v>
@@ -718,136 +718,136 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>0.361</v>
+        <v>0.393</v>
       </c>
       <c r="G2" t="n">
-        <v>-13.42126</v>
+        <v>-13.4091</v>
       </c>
       <c r="H2" t="n">
-        <v>5.062936</v>
+        <v>5.068114</v>
       </c>
       <c r="I2" t="n">
-        <v>5.008451462</v>
+        <v>4.973526001</v>
       </c>
       <c r="J2" t="n">
-        <v>-47.15045929</v>
+        <v>-47.02700806</v>
       </c>
       <c r="K2" t="n">
-        <v>0.1947240829467773</v>
+        <v>0.1871702671051025</v>
       </c>
       <c r="L2" t="n">
-        <v>5.06227397919</v>
+        <v>5.01795244217</v>
       </c>
       <c r="M2" t="n">
-        <v>-55.1005506516</v>
+        <v>-54.9861989021</v>
       </c>
       <c r="N2" t="n">
-        <v>-56.4154615402</v>
+        <v>-56.114086628</v>
       </c>
       <c r="O2" t="n">
-        <v>0.2165627479553223</v>
+        <v>0.2370998859405518</v>
       </c>
       <c r="P2" t="n">
-        <v>4.950866699</v>
+        <v>4.902143478</v>
       </c>
       <c r="Q2" t="n">
-        <v>-50.45854187</v>
+        <v>-50.4039917</v>
       </c>
       <c r="R2" t="n">
-        <v>0.1964597702026367</v>
+        <v>0.1929292678833008</v>
       </c>
       <c r="S2" t="n">
-        <v>5.01970767975</v>
+        <v>4.96074104309</v>
       </c>
       <c r="T2" t="n">
-        <v>-61.3057603836</v>
+        <v>-61.3053684235</v>
       </c>
       <c r="U2" t="n">
-        <v>-60.932847023</v>
+        <v>-60.9255847931</v>
       </c>
       <c r="V2" t="n">
-        <v>0.1904797554016113</v>
+        <v>0.1852684020996094</v>
       </c>
       <c r="W2" t="n">
-        <v>5.777019500732422</v>
+        <v>5.775356769561768</v>
       </c>
       <c r="X2" t="n">
         <v>2</v>
       </c>
       <c r="Y2" t="n">
-        <v>1.482</v>
+        <v>1.563</v>
       </c>
       <c r="Z2" t="n">
         <v>0</v>
       </c>
       <c r="AA2" t="n">
-        <v>5.007064819</v>
+        <v>4.969364166</v>
       </c>
       <c r="AB2" t="n">
-        <v>-50.36642456</v>
+        <v>-50.12388611</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.3049790859222412</v>
+        <v>0.3214728832244873</v>
       </c>
       <c r="AD2" t="n">
-        <v>5.0711555481</v>
+        <v>5.01970291138</v>
       </c>
       <c r="AE2" t="n">
-        <v>-56.6167411804</v>
+        <v>-56.5685920715</v>
       </c>
       <c r="AF2" t="n">
-        <v>-56.7238578796</v>
+        <v>-56.6907081604</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.1858468055725098</v>
+        <v>0.1915898323059082</v>
       </c>
       <c r="AH2" t="n">
-        <v>10.11187028884888</v>
+        <v>10.32633566856384</v>
       </c>
       <c r="AI2" t="n">
         <v>1</v>
       </c>
       <c r="AJ2" t="n">
-        <v>1.087</v>
+        <v>1.089</v>
       </c>
       <c r="AK2" t="n">
         <v>0</v>
       </c>
       <c r="AL2" t="n">
-        <v>5.01675415</v>
+        <v>4.983222961</v>
       </c>
       <c r="AM2" t="n">
-        <v>-50.23455048</v>
+        <v>-50.0286026</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.3202226161956787</v>
+        <v>0.3172593116760254</v>
       </c>
       <c r="AO2" t="n">
-        <v>5.08247852325</v>
+        <v>5.03259134293</v>
       </c>
       <c r="AP2" t="n">
-        <v>-60.1557283401</v>
+        <v>-60.1378731728</v>
       </c>
       <c r="AQ2" t="n">
-        <v>-60.3440828323</v>
+        <v>-60.3335328102</v>
       </c>
       <c r="AR2" t="n">
-        <v>0.1942791938781738</v>
+        <v>0.1960489749908447</v>
       </c>
       <c r="AS2" t="n">
-        <v>20.01556420326233</v>
+        <v>20.2311418056488</v>
       </c>
       <c r="AT2" t="n">
         <v>1</v>
       </c>
       <c r="AU2" t="n">
-        <v>1.137</v>
+        <v>1.252</v>
       </c>
       <c r="AV2" t="n">
         <v>0</v>
       </c>
       <c r="AW2" t="n">
-        <v>36.414</v>
+        <v>36.85</v>
       </c>
       <c r="AX2" s="2" t="inlineStr">
         <is>
@@ -860,13 +860,13 @@
     </row>
     <row r="3" ht="60" customHeight="1">
       <c r="A3" t="n">
-        <v>4.602265357971191</v>
+        <v>4.295692920684814</v>
       </c>
       <c r="B3" t="n">
-        <v>9.672922611236572</v>
+        <v>12.95009994506836</v>
       </c>
       <c r="C3" t="n">
-        <v>2.05</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
         <v>5</v>
@@ -875,136 +875,136 @@
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0.394</v>
+        <v>0.352</v>
       </c>
       <c r="G3" t="n">
-        <v>-13.37907</v>
+        <v>-12.80008</v>
       </c>
       <c r="H3" t="n">
-        <v>5.057403</v>
+        <v>5.024055</v>
       </c>
       <c r="I3" t="n">
-        <v>4.994890213</v>
+        <v>4.927913666</v>
       </c>
       <c r="J3" t="n">
-        <v>-50.44102478</v>
+        <v>-50.06105423</v>
       </c>
       <c r="K3" t="n">
-        <v>0.1933181285858154</v>
+        <v>0.1960487365722656</v>
       </c>
       <c r="L3" t="n">
-        <v>5.09518146515</v>
+        <v>5.00654697418</v>
       </c>
       <c r="M3" t="n">
-        <v>-60.6435899734</v>
+        <v>-60.3990488052</v>
       </c>
       <c r="N3" t="n">
-        <v>-60.4626893997</v>
+        <v>-61.2072763443</v>
       </c>
       <c r="O3" t="n">
-        <v>0.2783999443054199</v>
+        <v>0.2091443538665771</v>
       </c>
       <c r="P3" t="n">
-        <v>4.987430573</v>
+        <v>4.925983429</v>
       </c>
       <c r="Q3" t="n">
-        <v>-50.25976562</v>
+        <v>-50.04518509</v>
       </c>
       <c r="R3" t="n">
-        <v>0.1970160007476807</v>
+        <v>0.1975250244140625</v>
       </c>
       <c r="S3" t="n">
-        <v>5.07323026657</v>
+        <v>5.01486253738</v>
       </c>
       <c r="T3" t="n">
-        <v>-60.5573763847</v>
+        <v>-60.3891682625</v>
       </c>
       <c r="U3" t="n">
-        <v>-60.497607708</v>
+        <v>-61.2270207405</v>
       </c>
       <c r="V3" t="n">
-        <v>0.194901704788208</v>
+        <v>0.1903145313262939</v>
       </c>
       <c r="W3" t="n">
-        <v>2.926397562026978</v>
+        <v>3.019399642944336</v>
       </c>
       <c r="X3" t="n">
         <v>1</v>
       </c>
       <c r="Y3" t="n">
-        <v>1.163</v>
+        <v>1.28</v>
       </c>
       <c r="Z3" t="n">
         <v>0</v>
       </c>
       <c r="AA3" t="n">
-        <v>4.996162415</v>
+        <v>4.929424286</v>
       </c>
       <c r="AB3" t="n">
-        <v>-50.01766968</v>
+        <v>-49.52594757</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.3153629302978516</v>
+        <v>0.3138315677642822</v>
       </c>
       <c r="AD3" t="n">
-        <v>5.07546520233</v>
+        <v>5.01384782791</v>
       </c>
       <c r="AE3" t="n">
-        <v>-56.1423521042</v>
+        <v>-55.5860295296</v>
       </c>
       <c r="AF3" t="n">
-        <v>-56.4611463547</v>
+        <v>-55.7514500618</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.189298152923584</v>
+        <v>0.1920692920684814</v>
       </c>
       <c r="AH3" t="n">
-        <v>10.32540392875671</v>
+        <v>10.48429465293884</v>
       </c>
       <c r="AI3" t="n">
         <v>1</v>
       </c>
       <c r="AJ3" t="n">
-        <v>1.098</v>
+        <v>1.214</v>
       </c>
       <c r="AK3" t="n">
         <v>0</v>
       </c>
       <c r="AL3" t="n">
-        <v>4.996091843</v>
+        <v>4.940135956</v>
       </c>
       <c r="AM3" t="n">
-        <v>-50.33031464</v>
+        <v>-50.07219696</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.3131294250488281</v>
+        <v>0.3605415821075439</v>
       </c>
       <c r="AO3" t="n">
-        <v>5.07785367966</v>
+        <v>5.03083229065</v>
       </c>
       <c r="AP3" t="n">
-        <v>-59.9380526543</v>
+        <v>-60.4961071014</v>
       </c>
       <c r="AQ3" t="n">
-        <v>-60.2150263786</v>
+        <v>-61.4769763947</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.186826229095459</v>
+        <v>0.2140405178070068</v>
       </c>
       <c r="AS3" t="n">
-        <v>18.79442763328552</v>
+        <v>19.07639932632446</v>
       </c>
       <c r="AT3" t="n">
         <v>1</v>
       </c>
       <c r="AU3" t="n">
-        <v>1.222</v>
+        <v>1.128</v>
       </c>
       <c r="AV3" t="n">
         <v>0</v>
       </c>
       <c r="AW3" t="n">
-        <v>32.614</v>
+        <v>33.095</v>
       </c>
       <c r="AX3" s="2" t="inlineStr">
         <is>
@@ -1063,7 +1063,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4.602265357971191</v>
+        <v>4.295692920684814</v>
       </c>
     </row>
     <row r="4">
@@ -1073,7 +1073,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4.602265357971191</v>
+        <v>4.295692920684814</v>
       </c>
     </row>
     <row r="5">
@@ -1083,7 +1083,7 @@
         </is>
       </c>
       <c r="B5" s="4" t="n">
-        <v>4.602265357971191</v>
+        <v>4.295692920684814</v>
       </c>
     </row>
     <row r="6">
@@ -1093,7 +1093,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>9.672922611236572</v>
+        <v>12.95009994506836</v>
       </c>
     </row>
     <row r="7">
@@ -1103,7 +1103,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>9.672922611236572</v>
+        <v>12.95009994506836</v>
       </c>
     </row>
     <row r="8">
@@ -1113,7 +1113,7 @@
         </is>
       </c>
       <c r="B8" s="4" t="n">
-        <v>9.672922611236572</v>
+        <v>12.95009994506836</v>
       </c>
     </row>
     <row r="9">
@@ -1123,7 +1123,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2.05</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -1143,7 +1143,7 @@
         </is>
       </c>
       <c r="B11" s="4" t="n">
-        <v>2.025</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="12">
@@ -1213,7 +1213,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.394</v>
+        <v>0.393</v>
       </c>
     </row>
     <row r="19">
@@ -1223,7 +1223,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.361</v>
+        <v>0.352</v>
       </c>
     </row>
     <row r="20">
@@ -1233,7 +1233,7 @@
         </is>
       </c>
       <c r="B20" s="4" t="n">
-        <v>0.3775</v>
+        <v>0.3725</v>
       </c>
     </row>
     <row r="21">
@@ -1243,7 +1243,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-13.37907</v>
+        <v>-12.80008</v>
       </c>
     </row>
     <row r="22">
@@ -1253,7 +1253,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-13.42126</v>
+        <v>-13.4091</v>
       </c>
     </row>
     <row r="23">
@@ -1263,7 +1263,7 @@
         </is>
       </c>
       <c r="B23" s="4" t="n">
-        <v>-13.400165</v>
+        <v>-13.10459</v>
       </c>
     </row>
     <row r="24">
@@ -1273,7 +1273,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>5.062936</v>
+        <v>5.068114</v>
       </c>
     </row>
     <row r="25">
@@ -1283,7 +1283,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>5.057403</v>
+        <v>5.024055</v>
       </c>
     </row>
     <row r="26">
@@ -1293,7 +1293,7 @@
         </is>
       </c>
       <c r="B26" s="4" t="n">
-        <v>5.0601695</v>
+        <v>5.046084499999999</v>
       </c>
     </row>
     <row r="27">
@@ -1303,7 +1303,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>5.008451462</v>
+        <v>4.973526001</v>
       </c>
     </row>
     <row r="28">
@@ -1313,7 +1313,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>4.994890213</v>
+        <v>4.927913666</v>
       </c>
     </row>
     <row r="29">
@@ -1323,7 +1323,7 @@
         </is>
       </c>
       <c r="B29" s="4" t="n">
-        <v>5.0016708375</v>
+        <v>4.9507198335</v>
       </c>
     </row>
     <row r="30">
@@ -1333,7 +1333,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-47.15045929</v>
+        <v>-47.02700806</v>
       </c>
     </row>
     <row r="31">
@@ -1343,7 +1343,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-50.44102478</v>
+        <v>-50.06105423</v>
       </c>
     </row>
     <row r="32">
@@ -1353,7 +1353,7 @@
         </is>
       </c>
       <c r="B32" s="4" t="n">
-        <v>-48.795742035</v>
+        <v>-48.54403114500001</v>
       </c>
     </row>
     <row r="33">
@@ -1363,7 +1363,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.1947240829467773</v>
+        <v>0.1960487365722656</v>
       </c>
     </row>
     <row r="34">
@@ -1373,7 +1373,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.1933181285858154</v>
+        <v>0.1871702671051025</v>
       </c>
     </row>
     <row r="35">
@@ -1383,7 +1383,7 @@
         </is>
       </c>
       <c r="B35" s="4" t="n">
-        <v>0.1940211057662964</v>
+        <v>0.1916095018386841</v>
       </c>
     </row>
     <row r="36">
@@ -1393,7 +1393,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>5.09518146515</v>
+        <v>5.01795244217</v>
       </c>
     </row>
     <row r="37">
@@ -1403,7 +1403,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>5.06227397919</v>
+        <v>5.00654697418</v>
       </c>
     </row>
     <row r="38">
@@ -1413,7 +1413,7 @@
         </is>
       </c>
       <c r="B38" s="4" t="n">
-        <v>5.07872772217</v>
+        <v>5.012249708175</v>
       </c>
     </row>
     <row r="39">
@@ -1423,7 +1423,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>-55.1005506516</v>
+        <v>-54.9861989021</v>
       </c>
     </row>
     <row r="40">
@@ -1433,7 +1433,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>-60.6435899734</v>
+        <v>-60.3990488052</v>
       </c>
     </row>
     <row r="41">
@@ -1443,7 +1443,7 @@
         </is>
       </c>
       <c r="B41" s="4" t="n">
-        <v>-57.8720703125</v>
+        <v>-57.69262385365001</v>
       </c>
     </row>
     <row r="42">
@@ -1453,7 +1453,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>-56.4154615402</v>
+        <v>-56.114086628</v>
       </c>
     </row>
     <row r="43">
@@ -1463,7 +1463,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>-60.4626893997</v>
+        <v>-61.2072763443</v>
       </c>
     </row>
     <row r="44">
@@ -1473,7 +1473,7 @@
         </is>
       </c>
       <c r="B44" s="4" t="n">
-        <v>-58.43907546995</v>
+        <v>-58.66068148615</v>
       </c>
     </row>
     <row r="45">
@@ -1483,7 +1483,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.2783999443054199</v>
+        <v>0.2370998859405518</v>
       </c>
     </row>
     <row r="46">
@@ -1493,7 +1493,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.2165627479553223</v>
+        <v>0.2091443538665771</v>
       </c>
     </row>
     <row r="47">
@@ -1503,7 +1503,7 @@
         </is>
       </c>
       <c r="B47" s="4" t="n">
-        <v>0.2474813461303711</v>
+        <v>0.2231221199035645</v>
       </c>
     </row>
     <row r="48">
@@ -1513,7 +1513,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>4.987430573</v>
+        <v>4.925983429</v>
       </c>
     </row>
     <row r="49">
@@ -1523,7 +1523,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>4.950866699</v>
+        <v>4.902143478</v>
       </c>
     </row>
     <row r="50">
@@ -1533,7 +1533,7 @@
         </is>
       </c>
       <c r="B50" s="4" t="n">
-        <v>4.969148636</v>
+        <v>4.914063453500001</v>
       </c>
     </row>
     <row r="51">
@@ -1543,7 +1543,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>-50.25976562</v>
+        <v>-50.04518509</v>
       </c>
     </row>
     <row r="52">
@@ -1553,7 +1553,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>-50.45854187</v>
+        <v>-50.4039917</v>
       </c>
     </row>
     <row r="53">
@@ -1563,7 +1563,7 @@
         </is>
       </c>
       <c r="B53" s="4" t="n">
-        <v>-50.359153745</v>
+        <v>-50.224588395</v>
       </c>
     </row>
     <row r="54">
@@ -1573,7 +1573,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.1970160007476807</v>
+        <v>0.1975250244140625</v>
       </c>
     </row>
     <row r="55">
@@ -1583,7 +1583,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.1964597702026367</v>
+        <v>0.1929292678833008</v>
       </c>
     </row>
     <row r="56">
@@ -1593,7 +1593,7 @@
         </is>
       </c>
       <c r="B56" s="4" t="n">
-        <v>0.1967378854751587</v>
+        <v>0.1952271461486816</v>
       </c>
     </row>
     <row r="57">
@@ -1603,7 +1603,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>5.07323026657</v>
+        <v>5.01486253738</v>
       </c>
     </row>
     <row r="58">
@@ -1613,7 +1613,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>5.01970767975</v>
+        <v>4.96074104309</v>
       </c>
     </row>
     <row r="59">
@@ -1623,7 +1623,7 @@
         </is>
       </c>
       <c r="B59" s="4" t="n">
-        <v>5.04646897316</v>
+        <v>4.987801790235</v>
       </c>
     </row>
     <row r="60">
@@ -1633,7 +1633,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>-60.5573763847</v>
+        <v>-60.3891682625</v>
       </c>
     </row>
     <row r="61">
@@ -1643,7 +1643,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>-61.3057603836</v>
+        <v>-61.3053684235</v>
       </c>
     </row>
     <row r="62">
@@ -1653,7 +1653,7 @@
         </is>
       </c>
       <c r="B62" s="4" t="n">
-        <v>-60.93156838415</v>
+        <v>-60.847268343</v>
       </c>
     </row>
     <row r="63">
@@ -1663,7 +1663,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>-60.497607708</v>
+        <v>-60.9255847931</v>
       </c>
     </row>
     <row r="64">
@@ -1673,7 +1673,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>-60.932847023</v>
+        <v>-61.2270207405</v>
       </c>
     </row>
     <row r="65">
@@ -1683,7 +1683,7 @@
         </is>
       </c>
       <c r="B65" s="4" t="n">
-        <v>-60.7152273655</v>
+        <v>-61.0763027668</v>
       </c>
     </row>
     <row r="66">
@@ -1693,7 +1693,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.194901704788208</v>
+        <v>0.1903145313262939</v>
       </c>
     </row>
     <row r="67">
@@ -1703,7 +1703,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.1904797554016113</v>
+        <v>0.1852684020996094</v>
       </c>
     </row>
     <row r="68">
@@ -1713,7 +1713,7 @@
         </is>
       </c>
       <c r="B68" s="4" t="n">
-        <v>0.1926907300949097</v>
+        <v>0.1877914667129517</v>
       </c>
     </row>
     <row r="69">
@@ -1723,7 +1723,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>5.777019500732422</v>
+        <v>5.775356769561768</v>
       </c>
     </row>
     <row r="70">
@@ -1733,7 +1733,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>2.926397562026978</v>
+        <v>3.019399642944336</v>
       </c>
     </row>
     <row r="71">
@@ -1743,7 +1743,7 @@
         </is>
       </c>
       <c r="B71" s="4" t="n">
-        <v>4.3517085313797</v>
+        <v>4.397378206253052</v>
       </c>
     </row>
     <row r="72">
@@ -1783,7 +1783,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>1.482</v>
+        <v>1.563</v>
       </c>
     </row>
     <row r="76">
@@ -1793,7 +1793,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>1.163</v>
+        <v>1.28</v>
       </c>
     </row>
     <row r="77">
@@ -1803,7 +1803,7 @@
         </is>
       </c>
       <c r="B77" s="4" t="n">
-        <v>1.3225</v>
+        <v>1.4215</v>
       </c>
     </row>
     <row r="78">
@@ -1843,7 +1843,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>5.007064819</v>
+        <v>4.969364166</v>
       </c>
     </row>
     <row r="82">
@@ -1853,7 +1853,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>4.996162415</v>
+        <v>4.929424286</v>
       </c>
     </row>
     <row r="83">
@@ -1863,7 +1863,7 @@
         </is>
       </c>
       <c r="B83" s="4" t="n">
-        <v>5.001613617</v>
+        <v>4.949394226</v>
       </c>
     </row>
     <row r="84">
@@ -1873,7 +1873,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>-50.01766968</v>
+        <v>-49.52594757</v>
       </c>
     </row>
     <row r="85">
@@ -1883,7 +1883,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>-50.36642456</v>
+        <v>-50.12388611</v>
       </c>
     </row>
     <row r="86">
@@ -1893,7 +1893,7 @@
         </is>
       </c>
       <c r="B86" s="4" t="n">
-        <v>-50.19204712</v>
+        <v>-49.82491684</v>
       </c>
     </row>
     <row r="87">
@@ -1903,7 +1903,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0.3153629302978516</v>
+        <v>0.3214728832244873</v>
       </c>
     </row>
     <row r="88">
@@ -1913,7 +1913,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>0.3049790859222412</v>
+        <v>0.3138315677642822</v>
       </c>
     </row>
     <row r="89">
@@ -1923,7 +1923,7 @@
         </is>
       </c>
       <c r="B89" s="4" t="n">
-        <v>0.3101710081100464</v>
+        <v>0.3176522254943848</v>
       </c>
     </row>
     <row r="90">
@@ -1933,7 +1933,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>5.07546520233</v>
+        <v>5.01970291138</v>
       </c>
     </row>
     <row r="91">
@@ -1943,7 +1943,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>5.0711555481</v>
+        <v>5.01384782791</v>
       </c>
     </row>
     <row r="92">
@@ -1953,7 +1953,7 @@
         </is>
       </c>
       <c r="B92" s="4" t="n">
-        <v>5.073310375215</v>
+        <v>5.016775369645</v>
       </c>
     </row>
     <row r="93">
@@ -1963,7 +1963,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>-56.1423521042</v>
+        <v>-55.5860295296</v>
       </c>
     </row>
     <row r="94">
@@ -1973,7 +1973,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>-56.6167411804</v>
+        <v>-56.5685920715</v>
       </c>
     </row>
     <row r="95">
@@ -1983,7 +1983,7 @@
         </is>
       </c>
       <c r="B95" s="4" t="n">
-        <v>-56.3795466423</v>
+        <v>-56.07731080054999</v>
       </c>
     </row>
     <row r="96">
@@ -1993,7 +1993,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>-56.4611463547</v>
+        <v>-55.7514500618</v>
       </c>
     </row>
     <row r="97">
@@ -2003,7 +2003,7 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>-56.7238578796</v>
+        <v>-56.6907081604</v>
       </c>
     </row>
     <row r="98">
@@ -2013,7 +2013,7 @@
         </is>
       </c>
       <c r="B98" s="4" t="n">
-        <v>-56.59250211715</v>
+        <v>-56.2210791111</v>
       </c>
     </row>
     <row r="99">
@@ -2023,7 +2023,7 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>0.189298152923584</v>
+        <v>0.1920692920684814</v>
       </c>
     </row>
     <row r="100">
@@ -2033,7 +2033,7 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>0.1858468055725098</v>
+        <v>0.1915898323059082</v>
       </c>
     </row>
     <row r="101">
@@ -2043,7 +2043,7 @@
         </is>
       </c>
       <c r="B101" s="4" t="n">
-        <v>0.1875724792480469</v>
+        <v>0.1918295621871948</v>
       </c>
     </row>
     <row r="102">
@@ -2053,7 +2053,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>10.32540392875671</v>
+        <v>10.48429465293884</v>
       </c>
     </row>
     <row r="103">
@@ -2063,7 +2063,7 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>10.11187028884888</v>
+        <v>10.32633566856384</v>
       </c>
     </row>
     <row r="104">
@@ -2073,7 +2073,7 @@
         </is>
       </c>
       <c r="B104" s="4" t="n">
-        <v>10.2186371088028</v>
+        <v>10.40531516075134</v>
       </c>
     </row>
     <row r="105">
@@ -2113,7 +2113,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>1.098</v>
+        <v>1.214</v>
       </c>
     </row>
     <row r="109">
@@ -2123,7 +2123,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>1.087</v>
+        <v>1.089</v>
       </c>
     </row>
     <row r="110">
@@ -2133,7 +2133,7 @@
         </is>
       </c>
       <c r="B110" s="4" t="n">
-        <v>1.0925</v>
+        <v>1.1515</v>
       </c>
     </row>
     <row r="111">
@@ -2173,7 +2173,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>5.01675415</v>
+        <v>4.983222961</v>
       </c>
     </row>
     <row r="115">
@@ -2183,7 +2183,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>4.996091843</v>
+        <v>4.940135956</v>
       </c>
     </row>
     <row r="116">
@@ -2193,7 +2193,7 @@
         </is>
       </c>
       <c r="B116" s="4" t="n">
-        <v>5.0064229965</v>
+        <v>4.9616794585</v>
       </c>
     </row>
     <row r="117">
@@ -2203,7 +2203,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>-50.23455048</v>
+        <v>-50.0286026</v>
       </c>
     </row>
     <row r="118">
@@ -2213,7 +2213,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>-50.33031464</v>
+        <v>-50.07219696</v>
       </c>
     </row>
     <row r="119">
@@ -2223,7 +2223,7 @@
         </is>
       </c>
       <c r="B119" s="4" t="n">
-        <v>-50.28243256</v>
+        <v>-50.05039978</v>
       </c>
     </row>
     <row r="120">
@@ -2233,7 +2233,7 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>0.3202226161956787</v>
+        <v>0.3605415821075439</v>
       </c>
     </row>
     <row r="121">
@@ -2243,7 +2243,7 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>0.3131294250488281</v>
+        <v>0.3172593116760254</v>
       </c>
     </row>
     <row r="122">
@@ -2253,7 +2253,7 @@
         </is>
       </c>
       <c r="B122" s="4" t="n">
-        <v>0.3166760206222534</v>
+        <v>0.3389004468917847</v>
       </c>
     </row>
     <row r="123">
@@ -2263,7 +2263,7 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>5.08247852325</v>
+        <v>5.03259134293</v>
       </c>
     </row>
     <row r="124">
@@ -2273,7 +2273,7 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>5.07785367966</v>
+        <v>5.03083229065</v>
       </c>
     </row>
     <row r="125">
@@ -2283,7 +2283,7 @@
         </is>
       </c>
       <c r="B125" s="4" t="n">
-        <v>5.080166101454999</v>
+        <v>5.031711816790001</v>
       </c>
     </row>
     <row r="126">
@@ -2293,7 +2293,7 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>-59.9380526543</v>
+        <v>-60.1378731728</v>
       </c>
     </row>
     <row r="127">
@@ -2303,7 +2303,7 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>-60.1557283401</v>
+        <v>-60.4961071014</v>
       </c>
     </row>
     <row r="128">
@@ -2313,7 +2313,7 @@
         </is>
       </c>
       <c r="B128" s="4" t="n">
-        <v>-60.0468904972</v>
+        <v>-60.3169901371</v>
       </c>
     </row>
     <row r="129">
@@ -2323,7 +2323,7 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>-60.2150263786</v>
+        <v>-60.3335328102</v>
       </c>
     </row>
     <row r="130">
@@ -2333,7 +2333,7 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>-60.3440828323</v>
+        <v>-61.4769763947</v>
       </c>
     </row>
     <row r="131">
@@ -2343,7 +2343,7 @@
         </is>
       </c>
       <c r="B131" s="4" t="n">
-        <v>-60.27955460545</v>
+        <v>-60.90525460245</v>
       </c>
     </row>
     <row r="132">
@@ -2353,7 +2353,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>0.1942791938781738</v>
+        <v>0.2140405178070068</v>
       </c>
     </row>
     <row r="133">
@@ -2363,7 +2363,7 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>0.186826229095459</v>
+        <v>0.1960489749908447</v>
       </c>
     </row>
     <row r="134">
@@ -2373,7 +2373,7 @@
         </is>
       </c>
       <c r="B134" s="4" t="n">
-        <v>0.1905527114868164</v>
+        <v>0.2050447463989258</v>
       </c>
     </row>
     <row r="135">
@@ -2383,7 +2383,7 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>20.01556420326233</v>
+        <v>20.2311418056488</v>
       </c>
     </row>
     <row r="136">
@@ -2393,7 +2393,7 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>18.79442763328552</v>
+        <v>19.07639932632446</v>
       </c>
     </row>
     <row r="137">
@@ -2403,7 +2403,7 @@
         </is>
       </c>
       <c r="B137" s="4" t="n">
-        <v>19.40499591827393</v>
+        <v>19.65377056598663</v>
       </c>
     </row>
     <row r="138">
@@ -2443,7 +2443,7 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>1.222</v>
+        <v>1.252</v>
       </c>
     </row>
     <row r="142">
@@ -2453,7 +2453,7 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>1.137</v>
+        <v>1.128</v>
       </c>
     </row>
     <row r="143">
@@ -2463,7 +2463,7 @@
         </is>
       </c>
       <c r="B143" s="4" t="n">
-        <v>1.1795</v>
+        <v>1.19</v>
       </c>
     </row>
     <row r="144">
@@ -2503,7 +2503,7 @@
         </is>
       </c>
       <c r="B147" t="n">
-        <v>36.414</v>
+        <v>36.85</v>
       </c>
     </row>
     <row r="148">
@@ -2513,7 +2513,7 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>32.614</v>
+        <v>33.095</v>
       </c>
     </row>
     <row r="149">
@@ -2523,7 +2523,7 @@
         </is>
       </c>
       <c r="B149" s="4" t="n">
-        <v>34.514</v>
+        <v>34.9725</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20250918 issues remain, good push before edits.
</commit_message>
<xml_diff>
--- a/sweep_measurements.xlsx
+++ b/sweep_measurements.xlsx
@@ -703,10 +703,10 @@
     </row>
     <row r="2" ht="60" customHeight="1">
       <c r="A2" t="n">
-        <v>4.295692920684814</v>
+        <v>4.544441938400269</v>
       </c>
       <c r="B2" t="n">
-        <v>12.95009994506836</v>
+        <v>13.52477216720581</v>
       </c>
       <c r="C2" t="n">
         <v>2</v>
@@ -721,152 +721,152 @@
         <v>0.393</v>
       </c>
       <c r="G2" t="n">
-        <v>-13.4091</v>
+        <v>-13.43059</v>
       </c>
       <c r="H2" t="n">
-        <v>5.068114</v>
+        <v>5.085418</v>
       </c>
       <c r="I2" t="n">
-        <v>4.973526001</v>
+        <v>4.976383209</v>
       </c>
       <c r="J2" t="n">
-        <v>-47.02700806</v>
+        <v>-47.23838425</v>
       </c>
       <c r="K2" t="n">
-        <v>0.1871702671051025</v>
+        <v>0.1952049732208252</v>
       </c>
       <c r="L2" t="n">
-        <v>5.01795244217</v>
+        <v>5.02750635147</v>
       </c>
       <c r="M2" t="n">
-        <v>-54.9861989021</v>
+        <v>-55.1757493019</v>
       </c>
       <c r="N2" t="n">
-        <v>-56.114086628</v>
+        <v>-56.4646325111</v>
       </c>
       <c r="O2" t="n">
-        <v>0.2370998859405518</v>
+        <v>0.217111349105835</v>
       </c>
       <c r="P2" t="n">
-        <v>4.902143478</v>
+        <v>5.057008743</v>
       </c>
       <c r="Q2" t="n">
-        <v>-50.4039917</v>
+        <v>-50.3416481</v>
       </c>
       <c r="R2" t="n">
-        <v>0.1929292678833008</v>
+        <v>0.2275807857513428</v>
       </c>
       <c r="S2" t="n">
-        <v>4.96074104309</v>
+        <v>5.10628175735</v>
       </c>
       <c r="T2" t="n">
-        <v>-61.3053684235</v>
+        <v>-60.6061177254</v>
       </c>
       <c r="U2" t="n">
-        <v>-60.9255847931</v>
+        <v>-60.3064007759</v>
       </c>
       <c r="V2" t="n">
-        <v>0.1852684020996094</v>
+        <v>0.1907782554626465</v>
       </c>
       <c r="W2" t="n">
-        <v>5.775356769561768</v>
+        <v>6.935030698776245</v>
       </c>
       <c r="X2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y2" t="n">
-        <v>1.563</v>
+        <v>0</v>
       </c>
       <c r="Z2" t="n">
-        <v>0</v>
+        <v>2.638</v>
       </c>
       <c r="AA2" t="n">
-        <v>4.969364166</v>
+        <v>4.986499786</v>
       </c>
       <c r="AB2" t="n">
-        <v>-50.12388611</v>
+        <v>-50.09896851</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.3214728832244873</v>
+        <v>0.3401844501495361</v>
       </c>
       <c r="AD2" t="n">
-        <v>5.01970291138</v>
+        <v>5.03555059433</v>
       </c>
       <c r="AE2" t="n">
-        <v>-56.5685920715</v>
+        <v>-55.7622961998</v>
       </c>
       <c r="AF2" t="n">
-        <v>-56.6907081604</v>
+        <v>-55.8825850487</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.1915898323059082</v>
+        <v>0.1863663196563721</v>
       </c>
       <c r="AH2" t="n">
-        <v>10.32633566856384</v>
+        <v>11.75644135475159</v>
       </c>
       <c r="AI2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ2" t="n">
-        <v>1.089</v>
+        <v>0</v>
       </c>
       <c r="AK2" t="n">
-        <v>0</v>
+        <v>2.571</v>
       </c>
       <c r="AL2" t="n">
-        <v>4.983222961</v>
+        <v>4.984535217</v>
       </c>
       <c r="AM2" t="n">
-        <v>-50.0286026</v>
+        <v>-49.71195221</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.3172593116760254</v>
+        <v>0.3320817947387695</v>
       </c>
       <c r="AO2" t="n">
-        <v>5.03259134293</v>
+        <v>5.04499912262</v>
       </c>
       <c r="AP2" t="n">
-        <v>-60.1378731728</v>
+        <v>-58.7719774246</v>
       </c>
       <c r="AQ2" t="n">
-        <v>-60.3335328102</v>
+        <v>-58.9627084732</v>
       </c>
       <c r="AR2" t="n">
-        <v>0.1960489749908447</v>
+        <v>0.1902198791503906</v>
       </c>
       <c r="AS2" t="n">
-        <v>20.2311418056488</v>
+        <v>21.41870021820068</v>
       </c>
       <c r="AT2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU2" t="n">
-        <v>1.252</v>
+        <v>0</v>
       </c>
       <c r="AV2" t="n">
-        <v>0</v>
+        <v>2.566</v>
       </c>
       <c r="AW2" t="n">
-        <v>36.85</v>
+        <v>41.271</v>
       </c>
       <c r="AX2" s="2" t="inlineStr">
         <is>
           <t>The 5GNR waveform used in this test is a 10MHz UL, 30kHz SCS, 24QAM, 24RB, 0rbo configuration.
 This test utilizes the full 5G frame.
 The power servo is done after each DPD type to ensure accurate output power.
-The power servo uses the NRX power meter external sensors for power servo.</t>
+The power servo uses the NRX power meter and external sensors for power servo.</t>
         </is>
       </c>
     </row>
     <row r="3" ht="60" customHeight="1">
       <c r="A3" t="n">
-        <v>4.295692920684814</v>
+        <v>4.544441938400269</v>
       </c>
       <c r="B3" t="n">
-        <v>12.95009994506836</v>
+        <v>13.52477216720581</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>2.1</v>
       </c>
       <c r="D3" t="n">
         <v>5</v>
@@ -878,140 +878,140 @@
         <v>0.352</v>
       </c>
       <c r="G3" t="n">
-        <v>-12.80008</v>
+        <v>-13.47612</v>
       </c>
       <c r="H3" t="n">
-        <v>5.024055</v>
+        <v>5.036761</v>
       </c>
       <c r="I3" t="n">
-        <v>4.927913666</v>
+        <v>4.908203125</v>
       </c>
       <c r="J3" t="n">
-        <v>-50.06105423</v>
+        <v>-21.40676689</v>
       </c>
       <c r="K3" t="n">
-        <v>0.1960487365722656</v>
+        <v>0.1922016143798828</v>
       </c>
       <c r="L3" t="n">
-        <v>5.00654697418</v>
+        <v>4.97490406036</v>
       </c>
       <c r="M3" t="n">
-        <v>-60.3990488052</v>
+        <v>-55.1714296341</v>
       </c>
       <c r="N3" t="n">
-        <v>-61.2072763443</v>
+        <v>-56.3040742874</v>
       </c>
       <c r="O3" t="n">
-        <v>0.2091443538665771</v>
+        <v>0.1937520503997803</v>
       </c>
       <c r="P3" t="n">
-        <v>4.925983429</v>
+        <v>4.908157349</v>
       </c>
       <c r="Q3" t="n">
-        <v>-50.04518509</v>
+        <v>-21.40340424</v>
       </c>
       <c r="R3" t="n">
-        <v>0.1975250244140625</v>
+        <v>0.1980037689208984</v>
       </c>
       <c r="S3" t="n">
-        <v>5.01486253738</v>
+        <v>4.98175525665</v>
       </c>
       <c r="T3" t="n">
-        <v>-60.3891682625</v>
+        <v>-55.0589227676</v>
       </c>
       <c r="U3" t="n">
-        <v>-61.2270207405</v>
+        <v>-56.2393503189</v>
       </c>
       <c r="V3" t="n">
-        <v>0.1903145313262939</v>
+        <v>0.185863733291626</v>
       </c>
       <c r="W3" t="n">
-        <v>3.019399642944336</v>
+        <v>3.048375129699707</v>
       </c>
       <c r="X3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y3" t="n">
-        <v>1.28</v>
+        <v>0</v>
       </c>
       <c r="Z3" t="n">
-        <v>0</v>
+        <v>1.218</v>
       </c>
       <c r="AA3" t="n">
-        <v>4.929424286</v>
+        <v>5.009925842</v>
       </c>
       <c r="AB3" t="n">
-        <v>-49.52594757</v>
+        <v>-49.20523834</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.3138315677642822</v>
+        <v>0.3543787002563477</v>
       </c>
       <c r="AD3" t="n">
-        <v>5.01384782791</v>
+        <v>5.07956218719</v>
       </c>
       <c r="AE3" t="n">
-        <v>-55.5860295296</v>
+        <v>-54.4045591354</v>
       </c>
       <c r="AF3" t="n">
-        <v>-55.7514500618</v>
+        <v>-55.4119215012</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.1920692920684814</v>
+        <v>0.186917781829834</v>
       </c>
       <c r="AH3" t="n">
-        <v>10.48429465293884</v>
+        <v>11.80976676940918</v>
       </c>
       <c r="AI3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ3" t="n">
-        <v>1.214</v>
+        <v>0</v>
       </c>
       <c r="AK3" t="n">
-        <v>0</v>
+        <v>2.545</v>
       </c>
       <c r="AL3" t="n">
-        <v>4.940135956</v>
+        <v>5.010688782</v>
       </c>
       <c r="AM3" t="n">
-        <v>-50.07219696</v>
+        <v>-50.68193817</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.3605415821075439</v>
+        <v>0.3266315460205078</v>
       </c>
       <c r="AO3" t="n">
-        <v>5.03083229065</v>
+        <v>5.0837225914</v>
       </c>
       <c r="AP3" t="n">
-        <v>-60.4961071014</v>
+        <v>-60.4407744408</v>
       </c>
       <c r="AQ3" t="n">
-        <v>-61.4769763947</v>
+        <v>-60.4873366356</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.2140405178070068</v>
+        <v>0.1884052753448486</v>
       </c>
       <c r="AS3" t="n">
-        <v>19.07639932632446</v>
+        <v>20.66013479232788</v>
       </c>
       <c r="AT3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU3" t="n">
-        <v>1.128</v>
+        <v>0</v>
       </c>
       <c r="AV3" t="n">
-        <v>0</v>
+        <v>2.594</v>
       </c>
       <c r="AW3" t="n">
-        <v>33.095</v>
+        <v>36.657</v>
       </c>
       <c r="AX3" s="2" t="inlineStr">
         <is>
           <t>The 5GNR waveform used in this test is a 10MHz UL, 30kHz SCS, 24QAM, 24RB, 0rbo configuration.
 This test utilizes the full 5G frame.
 The power servo is done after each DPD type to ensure accurate output power.
-The power servo uses the NRX power meter external sensors for power servo.</t>
+The power servo uses the NRX power meter and external sensors for power servo.</t>
         </is>
       </c>
     </row>
@@ -1063,7 +1063,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4.295692920684814</v>
+        <v>4.544441938400269</v>
       </c>
     </row>
     <row r="4">
@@ -1073,7 +1073,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4.295692920684814</v>
+        <v>4.544441938400269</v>
       </c>
     </row>
     <row r="5">
@@ -1083,7 +1083,7 @@
         </is>
       </c>
       <c r="B5" s="4" t="n">
-        <v>4.295692920684814</v>
+        <v>4.544441938400269</v>
       </c>
     </row>
     <row r="6">
@@ -1093,7 +1093,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>12.95009994506836</v>
+        <v>13.52477216720581</v>
       </c>
     </row>
     <row r="7">
@@ -1103,7 +1103,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>12.95009994506836</v>
+        <v>13.52477216720581</v>
       </c>
     </row>
     <row r="8">
@@ -1113,7 +1113,7 @@
         </is>
       </c>
       <c r="B8" s="4" t="n">
-        <v>12.95009994506836</v>
+        <v>13.52477216720581</v>
       </c>
     </row>
     <row r="9">
@@ -1123,7 +1123,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="10">
@@ -1143,7 +1143,7 @@
         </is>
       </c>
       <c r="B11" s="4" t="n">
-        <v>2.5</v>
+        <v>2.05</v>
       </c>
     </row>
     <row r="12">
@@ -1243,7 +1243,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-12.80008</v>
+        <v>-13.43059</v>
       </c>
     </row>
     <row r="22">
@@ -1253,7 +1253,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-13.4091</v>
+        <v>-13.47612</v>
       </c>
     </row>
     <row r="23">
@@ -1263,7 +1263,7 @@
         </is>
       </c>
       <c r="B23" s="4" t="n">
-        <v>-13.10459</v>
+        <v>-13.453355</v>
       </c>
     </row>
     <row r="24">
@@ -1273,7 +1273,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>5.068114</v>
+        <v>5.085418</v>
       </c>
     </row>
     <row r="25">
@@ -1283,7 +1283,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>5.024055</v>
+        <v>5.036761</v>
       </c>
     </row>
     <row r="26">
@@ -1293,7 +1293,7 @@
         </is>
       </c>
       <c r="B26" s="4" t="n">
-        <v>5.046084499999999</v>
+        <v>5.0610895</v>
       </c>
     </row>
     <row r="27">
@@ -1303,7 +1303,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>4.973526001</v>
+        <v>4.976383209</v>
       </c>
     </row>
     <row r="28">
@@ -1313,7 +1313,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>4.927913666</v>
+        <v>4.908203125</v>
       </c>
     </row>
     <row r="29">
@@ -1323,7 +1323,7 @@
         </is>
       </c>
       <c r="B29" s="4" t="n">
-        <v>4.9507198335</v>
+        <v>4.942293167</v>
       </c>
     </row>
     <row r="30">
@@ -1333,7 +1333,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-47.02700806</v>
+        <v>-21.40676689</v>
       </c>
     </row>
     <row r="31">
@@ -1343,7 +1343,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-50.06105423</v>
+        <v>-47.23838425</v>
       </c>
     </row>
     <row r="32">
@@ -1353,7 +1353,7 @@
         </is>
       </c>
       <c r="B32" s="4" t="n">
-        <v>-48.54403114500001</v>
+        <v>-34.32257557</v>
       </c>
     </row>
     <row r="33">
@@ -1363,7 +1363,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.1960487365722656</v>
+        <v>0.1952049732208252</v>
       </c>
     </row>
     <row r="34">
@@ -1373,7 +1373,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.1871702671051025</v>
+        <v>0.1922016143798828</v>
       </c>
     </row>
     <row r="35">
@@ -1383,7 +1383,7 @@
         </is>
       </c>
       <c r="B35" s="4" t="n">
-        <v>0.1916095018386841</v>
+        <v>0.193703293800354</v>
       </c>
     </row>
     <row r="36">
@@ -1393,7 +1393,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>5.01795244217</v>
+        <v>5.02750635147</v>
       </c>
     </row>
     <row r="37">
@@ -1403,7 +1403,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>5.00654697418</v>
+        <v>4.97490406036</v>
       </c>
     </row>
     <row r="38">
@@ -1413,7 +1413,7 @@
         </is>
       </c>
       <c r="B38" s="4" t="n">
-        <v>5.012249708175</v>
+        <v>5.001205205914999</v>
       </c>
     </row>
     <row r="39">
@@ -1423,7 +1423,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>-54.9861989021</v>
+        <v>-55.1714296341</v>
       </c>
     </row>
     <row r="40">
@@ -1433,7 +1433,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>-60.3990488052</v>
+        <v>-55.1757493019</v>
       </c>
     </row>
     <row r="41">
@@ -1443,7 +1443,7 @@
         </is>
       </c>
       <c r="B41" s="4" t="n">
-        <v>-57.69262385365001</v>
+        <v>-55.173589468</v>
       </c>
     </row>
     <row r="42">
@@ -1453,7 +1453,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>-56.114086628</v>
+        <v>-56.3040742874</v>
       </c>
     </row>
     <row r="43">
@@ -1463,7 +1463,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>-61.2072763443</v>
+        <v>-56.4646325111</v>
       </c>
     </row>
     <row r="44">
@@ -1473,7 +1473,7 @@
         </is>
       </c>
       <c r="B44" s="4" t="n">
-        <v>-58.66068148615</v>
+        <v>-56.38435339925</v>
       </c>
     </row>
     <row r="45">
@@ -1483,7 +1483,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.2370998859405518</v>
+        <v>0.217111349105835</v>
       </c>
     </row>
     <row r="46">
@@ -1493,7 +1493,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.2091443538665771</v>
+        <v>0.1937520503997803</v>
       </c>
     </row>
     <row r="47">
@@ -1503,7 +1503,7 @@
         </is>
       </c>
       <c r="B47" s="4" t="n">
-        <v>0.2231221199035645</v>
+        <v>0.2054316997528076</v>
       </c>
     </row>
     <row r="48">
@@ -1513,7 +1513,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>4.925983429</v>
+        <v>5.057008743</v>
       </c>
     </row>
     <row r="49">
@@ -1523,7 +1523,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>4.902143478</v>
+        <v>4.908157349</v>
       </c>
     </row>
     <row r="50">
@@ -1533,7 +1533,7 @@
         </is>
       </c>
       <c r="B50" s="4" t="n">
-        <v>4.914063453500001</v>
+        <v>4.982583046</v>
       </c>
     </row>
     <row r="51">
@@ -1543,7 +1543,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>-50.04518509</v>
+        <v>-21.40340424</v>
       </c>
     </row>
     <row r="52">
@@ -1553,7 +1553,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>-50.4039917</v>
+        <v>-50.3416481</v>
       </c>
     </row>
     <row r="53">
@@ -1563,7 +1563,7 @@
         </is>
       </c>
       <c r="B53" s="4" t="n">
-        <v>-50.224588395</v>
+        <v>-35.87252617</v>
       </c>
     </row>
     <row r="54">
@@ -1573,7 +1573,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.1975250244140625</v>
+        <v>0.2275807857513428</v>
       </c>
     </row>
     <row r="55">
@@ -1583,7 +1583,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.1929292678833008</v>
+        <v>0.1980037689208984</v>
       </c>
     </row>
     <row r="56">
@@ -1593,7 +1593,7 @@
         </is>
       </c>
       <c r="B56" s="4" t="n">
-        <v>0.1952271461486816</v>
+        <v>0.2127922773361206</v>
       </c>
     </row>
     <row r="57">
@@ -1603,7 +1603,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>5.01486253738</v>
+        <v>5.10628175735</v>
       </c>
     </row>
     <row r="58">
@@ -1613,7 +1613,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>4.96074104309</v>
+        <v>4.98175525665</v>
       </c>
     </row>
     <row r="59">
@@ -1623,7 +1623,7 @@
         </is>
       </c>
       <c r="B59" s="4" t="n">
-        <v>4.987801790235</v>
+        <v>5.044018507</v>
       </c>
     </row>
     <row r="60">
@@ -1633,7 +1633,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>-60.3891682625</v>
+        <v>-55.0589227676</v>
       </c>
     </row>
     <row r="61">
@@ -1643,7 +1643,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>-61.3053684235</v>
+        <v>-60.6061177254</v>
       </c>
     </row>
     <row r="62">
@@ -1653,7 +1653,7 @@
         </is>
       </c>
       <c r="B62" s="4" t="n">
-        <v>-60.847268343</v>
+        <v>-57.8325202465</v>
       </c>
     </row>
     <row r="63">
@@ -1663,7 +1663,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>-60.9255847931</v>
+        <v>-56.2393503189</v>
       </c>
     </row>
     <row r="64">
@@ -1673,7 +1673,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>-61.2270207405</v>
+        <v>-60.3064007759</v>
       </c>
     </row>
     <row r="65">
@@ -1683,7 +1683,7 @@
         </is>
       </c>
       <c r="B65" s="4" t="n">
-        <v>-61.0763027668</v>
+        <v>-58.27287554740001</v>
       </c>
     </row>
     <row r="66">
@@ -1693,7 +1693,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.1903145313262939</v>
+        <v>0.1907782554626465</v>
       </c>
     </row>
     <row r="67">
@@ -1703,7 +1703,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.1852684020996094</v>
+        <v>0.185863733291626</v>
       </c>
     </row>
     <row r="68">
@@ -1713,7 +1713,7 @@
         </is>
       </c>
       <c r="B68" s="4" t="n">
-        <v>0.1877914667129517</v>
+        <v>0.1883209943771362</v>
       </c>
     </row>
     <row r="69">
@@ -1723,7 +1723,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>5.775356769561768</v>
+        <v>6.935030698776245</v>
       </c>
     </row>
     <row r="70">
@@ -1733,7 +1733,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>3.019399642944336</v>
+        <v>3.048375129699707</v>
       </c>
     </row>
     <row r="71">
@@ -1743,7 +1743,7 @@
         </is>
       </c>
       <c r="B71" s="4" t="n">
-        <v>4.397378206253052</v>
+        <v>4.991702914237976</v>
       </c>
     </row>
     <row r="72">
@@ -1753,7 +1753,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -1763,7 +1763,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -1773,7 +1773,7 @@
         </is>
       </c>
       <c r="B74" s="4" t="n">
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -1783,7 +1783,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>1.563</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -1793,7 +1793,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>1.28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -1803,7 +1803,7 @@
         </is>
       </c>
       <c r="B77" s="4" t="n">
-        <v>1.4215</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -1813,7 +1813,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0</v>
+        <v>2.638</v>
       </c>
     </row>
     <row r="79">
@@ -1823,7 +1823,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>0</v>
+        <v>1.218</v>
       </c>
     </row>
     <row r="80">
@@ -1833,7 +1833,7 @@
         </is>
       </c>
       <c r="B80" s="4" t="n">
-        <v>0</v>
+        <v>1.928</v>
       </c>
     </row>
     <row r="81">
@@ -1843,7 +1843,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>4.969364166</v>
+        <v>5.009925842</v>
       </c>
     </row>
     <row r="82">
@@ -1853,7 +1853,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>4.929424286</v>
+        <v>4.986499786</v>
       </c>
     </row>
     <row r="83">
@@ -1863,7 +1863,7 @@
         </is>
       </c>
       <c r="B83" s="4" t="n">
-        <v>4.949394226</v>
+        <v>4.998212814</v>
       </c>
     </row>
     <row r="84">
@@ -1873,7 +1873,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>-49.52594757</v>
+        <v>-49.20523834</v>
       </c>
     </row>
     <row r="85">
@@ -1883,7 +1883,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>-50.12388611</v>
+        <v>-50.09896851</v>
       </c>
     </row>
     <row r="86">
@@ -1893,7 +1893,7 @@
         </is>
       </c>
       <c r="B86" s="4" t="n">
-        <v>-49.82491684</v>
+        <v>-49.652103425</v>
       </c>
     </row>
     <row r="87">
@@ -1903,7 +1903,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0.3214728832244873</v>
+        <v>0.3543787002563477</v>
       </c>
     </row>
     <row r="88">
@@ -1913,7 +1913,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>0.3138315677642822</v>
+        <v>0.3401844501495361</v>
       </c>
     </row>
     <row r="89">
@@ -1923,7 +1923,7 @@
         </is>
       </c>
       <c r="B89" s="4" t="n">
-        <v>0.3176522254943848</v>
+        <v>0.3472815752029419</v>
       </c>
     </row>
     <row r="90">
@@ -1933,7 +1933,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>5.01970291138</v>
+        <v>5.07956218719</v>
       </c>
     </row>
     <row r="91">
@@ -1943,7 +1943,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>5.01384782791</v>
+        <v>5.03555059433</v>
       </c>
     </row>
     <row r="92">
@@ -1953,7 +1953,7 @@
         </is>
       </c>
       <c r="B92" s="4" t="n">
-        <v>5.016775369645</v>
+        <v>5.05755639076</v>
       </c>
     </row>
     <row r="93">
@@ -1963,7 +1963,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>-55.5860295296</v>
+        <v>-54.4045591354</v>
       </c>
     </row>
     <row r="94">
@@ -1973,7 +1973,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>-56.5685920715</v>
+        <v>-55.7622961998</v>
       </c>
     </row>
     <row r="95">
@@ -1983,7 +1983,7 @@
         </is>
       </c>
       <c r="B95" s="4" t="n">
-        <v>-56.07731080054999</v>
+        <v>-55.0834276676</v>
       </c>
     </row>
     <row r="96">
@@ -1993,7 +1993,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>-55.7514500618</v>
+        <v>-55.4119215012</v>
       </c>
     </row>
     <row r="97">
@@ -2003,7 +2003,7 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>-56.6907081604</v>
+        <v>-55.8825850487</v>
       </c>
     </row>
     <row r="98">
@@ -2013,7 +2013,7 @@
         </is>
       </c>
       <c r="B98" s="4" t="n">
-        <v>-56.2210791111</v>
+        <v>-55.64725327495</v>
       </c>
     </row>
     <row r="99">
@@ -2023,7 +2023,7 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>0.1920692920684814</v>
+        <v>0.186917781829834</v>
       </c>
     </row>
     <row r="100">
@@ -2033,7 +2033,7 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>0.1915898323059082</v>
+        <v>0.1863663196563721</v>
       </c>
     </row>
     <row r="101">
@@ -2043,7 +2043,7 @@
         </is>
       </c>
       <c r="B101" s="4" t="n">
-        <v>0.1918295621871948</v>
+        <v>0.186642050743103</v>
       </c>
     </row>
     <row r="102">
@@ -2053,7 +2053,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>10.48429465293884</v>
+        <v>11.80976676940918</v>
       </c>
     </row>
     <row r="103">
@@ -2063,7 +2063,7 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>10.32633566856384</v>
+        <v>11.75644135475159</v>
       </c>
     </row>
     <row r="104">
@@ -2073,7 +2073,7 @@
         </is>
       </c>
       <c r="B104" s="4" t="n">
-        <v>10.40531516075134</v>
+        <v>11.78310406208038</v>
       </c>
     </row>
     <row r="105">
@@ -2083,7 +2083,7 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106">
@@ -2093,7 +2093,7 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107">
@@ -2103,7 +2103,7 @@
         </is>
       </c>
       <c r="B107" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108">
@@ -2113,7 +2113,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>1.214</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109">
@@ -2123,7 +2123,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>1.089</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110">
@@ -2133,7 +2133,7 @@
         </is>
       </c>
       <c r="B110" s="4" t="n">
-        <v>1.1515</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111">
@@ -2143,7 +2143,7 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>0</v>
+        <v>2.571</v>
       </c>
     </row>
     <row r="112">
@@ -2153,7 +2153,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>0</v>
+        <v>2.545</v>
       </c>
     </row>
     <row r="113">
@@ -2163,7 +2163,7 @@
         </is>
       </c>
       <c r="B113" s="4" t="n">
-        <v>0</v>
+        <v>2.558</v>
       </c>
     </row>
     <row r="114">
@@ -2173,7 +2173,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>4.983222961</v>
+        <v>5.010688782</v>
       </c>
     </row>
     <row r="115">
@@ -2183,7 +2183,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>4.940135956</v>
+        <v>4.984535217</v>
       </c>
     </row>
     <row r="116">
@@ -2193,7 +2193,7 @@
         </is>
       </c>
       <c r="B116" s="4" t="n">
-        <v>4.9616794585</v>
+        <v>4.9976119995</v>
       </c>
     </row>
     <row r="117">
@@ -2203,7 +2203,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>-50.0286026</v>
+        <v>-49.71195221</v>
       </c>
     </row>
     <row r="118">
@@ -2213,7 +2213,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>-50.07219696</v>
+        <v>-50.68193817</v>
       </c>
     </row>
     <row r="119">
@@ -2223,7 +2223,7 @@
         </is>
       </c>
       <c r="B119" s="4" t="n">
-        <v>-50.05039978</v>
+        <v>-50.19694519</v>
       </c>
     </row>
     <row r="120">
@@ -2233,7 +2233,7 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>0.3605415821075439</v>
+        <v>0.3320817947387695</v>
       </c>
     </row>
     <row r="121">
@@ -2243,7 +2243,7 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>0.3172593116760254</v>
+        <v>0.3266315460205078</v>
       </c>
     </row>
     <row r="122">
@@ -2253,7 +2253,7 @@
         </is>
       </c>
       <c r="B122" s="4" t="n">
-        <v>0.3389004468917847</v>
+        <v>0.3293566703796387</v>
       </c>
     </row>
     <row r="123">
@@ -2263,7 +2263,7 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>5.03259134293</v>
+        <v>5.0837225914</v>
       </c>
     </row>
     <row r="124">
@@ -2273,7 +2273,7 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>5.03083229065</v>
+        <v>5.04499912262</v>
       </c>
     </row>
     <row r="125">
@@ -2283,7 +2283,7 @@
         </is>
       </c>
       <c r="B125" s="4" t="n">
-        <v>5.031711816790001</v>
+        <v>5.06436085701</v>
       </c>
     </row>
     <row r="126">
@@ -2293,7 +2293,7 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>-60.1378731728</v>
+        <v>-58.7719774246</v>
       </c>
     </row>
     <row r="127">
@@ -2303,7 +2303,7 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>-60.4961071014</v>
+        <v>-60.4407744408</v>
       </c>
     </row>
     <row r="128">
@@ -2313,7 +2313,7 @@
         </is>
       </c>
       <c r="B128" s="4" t="n">
-        <v>-60.3169901371</v>
+        <v>-59.6063759327</v>
       </c>
     </row>
     <row r="129">
@@ -2323,7 +2323,7 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>-60.3335328102</v>
+        <v>-58.9627084732</v>
       </c>
     </row>
     <row r="130">
@@ -2333,7 +2333,7 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>-61.4769763947</v>
+        <v>-60.4873366356</v>
       </c>
     </row>
     <row r="131">
@@ -2343,7 +2343,7 @@
         </is>
       </c>
       <c r="B131" s="4" t="n">
-        <v>-60.90525460245</v>
+        <v>-59.7250225544</v>
       </c>
     </row>
     <row r="132">
@@ -2353,7 +2353,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>0.2140405178070068</v>
+        <v>0.1902198791503906</v>
       </c>
     </row>
     <row r="133">
@@ -2363,7 +2363,7 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>0.1960489749908447</v>
+        <v>0.1884052753448486</v>
       </c>
     </row>
     <row r="134">
@@ -2373,7 +2373,7 @@
         </is>
       </c>
       <c r="B134" s="4" t="n">
-        <v>0.2050447463989258</v>
+        <v>0.1893125772476196</v>
       </c>
     </row>
     <row r="135">
@@ -2383,7 +2383,7 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>20.2311418056488</v>
+        <v>21.41870021820068</v>
       </c>
     </row>
     <row r="136">
@@ -2393,7 +2393,7 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>19.07639932632446</v>
+        <v>20.66013479232788</v>
       </c>
     </row>
     <row r="137">
@@ -2403,7 +2403,7 @@
         </is>
       </c>
       <c r="B137" s="4" t="n">
-        <v>19.65377056598663</v>
+        <v>21.03941750526428</v>
       </c>
     </row>
     <row r="138">
@@ -2413,7 +2413,7 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139">
@@ -2423,7 +2423,7 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140">
@@ -2433,7 +2433,7 @@
         </is>
       </c>
       <c r="B140" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141">
@@ -2443,7 +2443,7 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>1.252</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142">
@@ -2453,7 +2453,7 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>1.128</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143">
@@ -2463,7 +2463,7 @@
         </is>
       </c>
       <c r="B143" s="4" t="n">
-        <v>1.19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144">
@@ -2473,7 +2473,7 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>0</v>
+        <v>2.594</v>
       </c>
     </row>
     <row r="145">
@@ -2483,7 +2483,7 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>0</v>
+        <v>2.566</v>
       </c>
     </row>
     <row r="146">
@@ -2493,7 +2493,7 @@
         </is>
       </c>
       <c r="B146" s="4" t="n">
-        <v>0</v>
+        <v>2.58</v>
       </c>
     </row>
     <row r="147">
@@ -2503,7 +2503,7 @@
         </is>
       </c>
       <c r="B147" t="n">
-        <v>36.85</v>
+        <v>41.271</v>
       </c>
     </row>
     <row r="148">
@@ -2513,7 +2513,7 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>33.095</v>
+        <v>36.657</v>
       </c>
     </row>
     <row r="149">
@@ -2523,7 +2523,7 @@
         </is>
       </c>
       <c r="B149" s="4" t="n">
-        <v>34.9725</v>
+        <v>38.964</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20250923 project is working well, commit to save a know good
</commit_message>
<xml_diff>
--- a/sweep_measurements.xlsx
+++ b/sweep_measurements.xlsx
@@ -441,7 +441,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AX3"/>
+  <dimension ref="A1:AX8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -701,75 +701,75 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="60" customHeight="1">
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" t="n">
-        <v>4.544441938400269</v>
+        <v>1.220230579376221</v>
       </c>
       <c r="B2" t="n">
-        <v>13.52477216720581</v>
+        <v>3.601427555084229</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>0.393</v>
+        <v>0.555</v>
       </c>
       <c r="G2" t="n">
-        <v>-13.43059</v>
+        <v>-10.99513</v>
       </c>
       <c r="H2" t="n">
-        <v>5.085418</v>
+        <v>5.929387</v>
       </c>
       <c r="I2" t="n">
-        <v>4.976383209</v>
+        <v>5.905197144</v>
       </c>
       <c r="J2" t="n">
-        <v>-47.23838425</v>
+        <v>-43.7933197</v>
       </c>
       <c r="K2" t="n">
-        <v>0.1952049732208252</v>
+        <v>0.1043274402618408</v>
       </c>
       <c r="L2" t="n">
-        <v>5.02750635147</v>
+        <v>5.93272781372</v>
       </c>
       <c r="M2" t="n">
-        <v>-55.1757493019</v>
+        <v>-51.6141395569</v>
       </c>
       <c r="N2" t="n">
-        <v>-56.4646325111</v>
+        <v>-53.0046730042</v>
       </c>
       <c r="O2" t="n">
-        <v>0.217111349105835</v>
+        <v>0.1998167037963867</v>
       </c>
       <c r="P2" t="n">
-        <v>5.057008743</v>
+        <v>5.971302032</v>
       </c>
       <c r="Q2" t="n">
-        <v>-50.3416481</v>
+        <v>-50.41112518</v>
       </c>
       <c r="R2" t="n">
-        <v>0.2275807857513428</v>
+        <v>0.0866706371307373</v>
       </c>
       <c r="S2" t="n">
-        <v>5.10628175735</v>
+        <v>6.04659557343</v>
       </c>
       <c r="T2" t="n">
-        <v>-60.6061177254</v>
+        <v>-49.6169271469</v>
       </c>
       <c r="U2" t="n">
-        <v>-60.3064007759</v>
+        <v>-52.4700574875</v>
       </c>
       <c r="V2" t="n">
-        <v>0.1907782554626465</v>
+        <v>0.1782207489013672</v>
       </c>
       <c r="W2" t="n">
-        <v>6.935030698776245</v>
+        <v>6.827713489532471</v>
       </c>
       <c r="X2" t="n">
         <v>0</v>
@@ -778,31 +778,31 @@
         <v>0</v>
       </c>
       <c r="Z2" t="n">
-        <v>2.638</v>
+        <v>0.409</v>
       </c>
       <c r="AA2" t="n">
-        <v>4.986499786</v>
+        <v>5.982486725</v>
       </c>
       <c r="AB2" t="n">
-        <v>-50.09896851</v>
+        <v>-49.02235031</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.3401844501495361</v>
+        <v>0.15743088722229</v>
       </c>
       <c r="AD2" t="n">
-        <v>5.03555059433</v>
+        <v>6.05910825729</v>
       </c>
       <c r="AE2" t="n">
-        <v>-55.7622961998</v>
+        <v>-48.4489855766</v>
       </c>
       <c r="AF2" t="n">
-        <v>-55.8825850487</v>
+        <v>-50.3370471001</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.1863663196563721</v>
+        <v>0.1763713359832764</v>
       </c>
       <c r="AH2" t="n">
-        <v>11.75644135475159</v>
+        <v>2.707039833068848</v>
       </c>
       <c r="AI2" t="n">
         <v>0</v>
@@ -811,31 +811,31 @@
         <v>0</v>
       </c>
       <c r="AK2" t="n">
-        <v>2.571</v>
+        <v>0.4</v>
       </c>
       <c r="AL2" t="n">
-        <v>4.984535217</v>
+        <v>5.914958954</v>
       </c>
       <c r="AM2" t="n">
-        <v>-49.71195221</v>
+        <v>-49.59848022</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.3320817947387695</v>
+        <v>0.1543612480163574</v>
       </c>
       <c r="AO2" t="n">
-        <v>5.04499912262</v>
+        <v>5.94747495651</v>
       </c>
       <c r="AP2" t="n">
-        <v>-58.7719774246</v>
+        <v>-59.9518580437</v>
       </c>
       <c r="AQ2" t="n">
-        <v>-58.9627084732</v>
+        <v>-60.6399531364</v>
       </c>
       <c r="AR2" t="n">
-        <v>0.1902198791503906</v>
+        <v>0.1940133571624756</v>
       </c>
       <c r="AS2" t="n">
-        <v>21.41870021820068</v>
+        <v>9.742092847824097</v>
       </c>
       <c r="AT2" t="n">
         <v>0</v>
@@ -844,89 +844,82 @@
         <v>0</v>
       </c>
       <c r="AV2" t="n">
-        <v>2.566</v>
+        <v>0.425</v>
       </c>
       <c r="AW2" t="n">
-        <v>41.271</v>
-      </c>
-      <c r="AX2" s="2" t="inlineStr">
-        <is>
-          <t>The 5GNR waveform used in this test is a 10MHz UL, 30kHz SCS, 24QAM, 24RB, 0rbo configuration.
-This test utilizes the full 5G frame.
-The power servo is done after each DPD type to ensure accurate output power.
-The power servo uses the NRX power meter and external sensors for power servo.</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="60" customHeight="1">
+        <v>27.307</v>
+      </c>
+      <c r="AX2" s="2" t="inlineStr"/>
+    </row>
+    <row r="3" ht="15" customHeight="1">
       <c r="A3" t="n">
-        <v>4.544441938400269</v>
+        <v>1.220230579376221</v>
       </c>
       <c r="B3" t="n">
-        <v>13.52477216720581</v>
+        <v>3.601427555084229</v>
       </c>
       <c r="C3" t="n">
-        <v>2.1</v>
+        <v>4.1</v>
       </c>
       <c r="D3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0.352</v>
+        <v>0.403</v>
       </c>
       <c r="G3" t="n">
-        <v>-13.47612</v>
+        <v>-10.71387</v>
       </c>
       <c r="H3" t="n">
-        <v>5.036761</v>
+        <v>6.003528</v>
       </c>
       <c r="I3" t="n">
-        <v>4.908203125</v>
+        <v>5.952327728</v>
       </c>
       <c r="J3" t="n">
-        <v>-21.40676689</v>
+        <v>-43.88660812</v>
       </c>
       <c r="K3" t="n">
-        <v>0.1922016143798828</v>
+        <v>0.1090087890625</v>
       </c>
       <c r="L3" t="n">
-        <v>4.97490406036</v>
+        <v>6.02062749863</v>
       </c>
       <c r="M3" t="n">
-        <v>-55.1714296341</v>
+        <v>-51.8926329613</v>
       </c>
       <c r="N3" t="n">
-        <v>-56.3040742874</v>
+        <v>-53.2699217796</v>
       </c>
       <c r="O3" t="n">
-        <v>0.1937520503997803</v>
+        <v>0.192603588104248</v>
       </c>
       <c r="P3" t="n">
-        <v>4.908157349</v>
+        <v>5.913562775</v>
       </c>
       <c r="Q3" t="n">
-        <v>-21.40340424</v>
+        <v>-50.61495209</v>
       </c>
       <c r="R3" t="n">
-        <v>0.1980037689208984</v>
+        <v>0.09663581848144531</v>
       </c>
       <c r="S3" t="n">
-        <v>4.98175525665</v>
+        <v>6.02402734756</v>
       </c>
       <c r="T3" t="n">
-        <v>-55.0589227676</v>
+        <v>-50.4292626381</v>
       </c>
       <c r="U3" t="n">
-        <v>-56.2393503189</v>
+        <v>-52.0804390907</v>
       </c>
       <c r="V3" t="n">
-        <v>0.185863733291626</v>
+        <v>0.1820697784423828</v>
       </c>
       <c r="W3" t="n">
-        <v>3.048375129699707</v>
+        <v>6.274100780487061</v>
       </c>
       <c r="X3" t="n">
         <v>0</v>
@@ -935,31 +928,31 @@
         <v>0</v>
       </c>
       <c r="Z3" t="n">
-        <v>1.218</v>
+        <v>0.181</v>
       </c>
       <c r="AA3" t="n">
-        <v>5.009925842</v>
+        <v>5.911529541</v>
       </c>
       <c r="AB3" t="n">
-        <v>-49.20523834</v>
+        <v>-48.9655838</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.3543787002563477</v>
+        <v>0.1908462047576904</v>
       </c>
       <c r="AD3" t="n">
-        <v>5.07956218719</v>
+        <v>6.0308675766</v>
       </c>
       <c r="AE3" t="n">
-        <v>-54.4045591354</v>
+        <v>-48.5944280624</v>
       </c>
       <c r="AF3" t="n">
-        <v>-55.4119215012</v>
+        <v>-50.3751173019</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.186917781829834</v>
+        <v>0.1806857585906982</v>
       </c>
       <c r="AH3" t="n">
-        <v>11.80976676940918</v>
+        <v>2.836046457290649</v>
       </c>
       <c r="AI3" t="n">
         <v>0</v>
@@ -968,31 +961,31 @@
         <v>0</v>
       </c>
       <c r="AK3" t="n">
-        <v>2.545</v>
+        <v>0.43</v>
       </c>
       <c r="AL3" t="n">
-        <v>5.010688782</v>
+        <v>5.951593399</v>
       </c>
       <c r="AM3" t="n">
-        <v>-50.68193817</v>
+        <v>-49.17251587</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.3266315460205078</v>
+        <v>0.1651663780212402</v>
       </c>
       <c r="AO3" t="n">
-        <v>5.0837225914</v>
+        <v>6.03072452545</v>
       </c>
       <c r="AP3" t="n">
-        <v>-60.4407744408</v>
+        <v>-59.9182367325</v>
       </c>
       <c r="AQ3" t="n">
-        <v>-60.4873366356</v>
+        <v>-60.3616609573</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.1884052753448486</v>
+        <v>0.1942462921142578</v>
       </c>
       <c r="AS3" t="n">
-        <v>20.66013479232788</v>
+        <v>9.311590671539307</v>
       </c>
       <c r="AT3" t="n">
         <v>0</v>
@@ -1001,19 +994,762 @@
         <v>0</v>
       </c>
       <c r="AV3" t="n">
-        <v>2.594</v>
+        <v>0.446</v>
       </c>
       <c r="AW3" t="n">
-        <v>36.657</v>
-      </c>
-      <c r="AX3" s="2" t="inlineStr">
-        <is>
-          <t>The 5GNR waveform used in this test is a 10MHz UL, 30kHz SCS, 24QAM, 24RB, 0rbo configuration.
-This test utilizes the full 5G frame.
-The power servo is done after each DPD type to ensure accurate output power.
-The power servo uses the NRX power meter and external sensors for power servo.</t>
-        </is>
-      </c>
+        <v>26.24</v>
+      </c>
+      <c r="AX3" s="2" t="inlineStr"/>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" t="n">
+        <v>1.220230579376221</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3.601427555084229</v>
+      </c>
+      <c r="C4" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>6</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-10.82424</v>
+      </c>
+      <c r="H4" t="n">
+        <v>6.005121</v>
+      </c>
+      <c r="I4" t="n">
+        <v>5.904348373</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-44.29456329</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.07992815971374512</v>
+      </c>
+      <c r="L4" t="n">
+        <v>5.99493026733</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-52.0992126465</v>
+      </c>
+      <c r="N4" t="n">
+        <v>-53.5028305054</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.186129093170166</v>
+      </c>
+      <c r="P4" t="n">
+        <v>5.870141983</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-50.57678986</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.07984685897827148</v>
+      </c>
+      <c r="S4" t="n">
+        <v>6.00778341293</v>
+      </c>
+      <c r="T4" t="n">
+        <v>-49.603662014</v>
+      </c>
+      <c r="U4" t="n">
+        <v>-52.3552794456</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0.1545419692993164</v>
+      </c>
+      <c r="W4" t="n">
+        <v>7.262543916702271</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0.188</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>5.975738525</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>-49.47615814</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>0.1377959251403809</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>6.11211681366</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>-48.6733617783</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>-50.8653478622</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>0.1530272960662842</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>2.78815746307373</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>0.411</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>5.913640976</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>-50.08543396</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>0.1237905025482178</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>5.99904155731</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>-60.6964216232</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>-59.9297742844</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>0.1895630359649658</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>9.392547369003296</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>0.403</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>27.075</v>
+      </c>
+      <c r="AX4" s="2" t="inlineStr"/>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" t="n">
+        <v>1.220230579376221</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3.601427555084229</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.606</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-10.96826</v>
+      </c>
+      <c r="H5" t="n">
+        <v>6.032585</v>
+      </c>
+      <c r="I5" t="n">
+        <v>5.959341049</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-44.20947647</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.09226107597351074</v>
+      </c>
+      <c r="L5" t="n">
+        <v>6.04576396942</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-51.904009819</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-53.4327001572</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.1979174613952637</v>
+      </c>
+      <c r="P5" t="n">
+        <v>5.921918869</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-50.83035278</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.04189252853393555</v>
+      </c>
+      <c r="S5" t="n">
+        <v>6.05037403107</v>
+      </c>
+      <c r="T5" t="n">
+        <v>-49.6174402237</v>
+      </c>
+      <c r="U5" t="n">
+        <v>-52.6674547195</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0.1787078380584717</v>
+      </c>
+      <c r="W5" t="n">
+        <v>7.230472564697266</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.176</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>5.922689438</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>-49.75502396</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>0.1813395023345947</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>6.05016994476</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>-48.7619047165</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>-50.5073003769</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>0.1777670383453369</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>2.725986242294312</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>0.384</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>5.953754425</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>-50.27392578</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>0.1299064159393311</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>6.04695129395</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>-60.7487335205</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>-61.0186157227</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>0.1886463165283203</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>9.319432497024536</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>0.423</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>27.224</v>
+      </c>
+      <c r="AX5" s="2" t="inlineStr"/>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" t="n">
+        <v>1.220230579376221</v>
+      </c>
+      <c r="B6" t="n">
+        <v>3.601427555084229</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="D6" t="n">
+        <v>6</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.594</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-10.93479</v>
+      </c>
+      <c r="H6" t="n">
+        <v>5.937651</v>
+      </c>
+      <c r="I6" t="n">
+        <v>5.923822403</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-43.79166031</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.1474802494049072</v>
+      </c>
+      <c r="L6" t="n">
+        <v>5.96760511398</v>
+      </c>
+      <c r="M6" t="n">
+        <v>-51.4035868645</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-52.8622965813</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.1923964023590088</v>
+      </c>
+      <c r="P6" t="n">
+        <v>5.884895325</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-50.72265244</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.08623671531677246</v>
+      </c>
+      <c r="S6" t="n">
+        <v>5.97079944611</v>
+      </c>
+      <c r="T6" t="n">
+        <v>-49.2488260269</v>
+      </c>
+      <c r="U6" t="n">
+        <v>-52.2822999954</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.1858205795288086</v>
+      </c>
+      <c r="W6" t="n">
+        <v>7.333505630493164</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0.195</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>5.985588074</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>-49.01224136</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>0.1716275215148926</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>6.06830358505</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>-48.481107235</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>-50.1791052818</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>0.1749708652496338</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>2.733812808990479</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>0.406</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>5.921880722</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>-49.69962311</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>0.1499216556549072</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>5.96842288971</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>-59.8529634476</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>-60.2399606705</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>0.1987082958221436</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>9.361552000045776</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>0.446</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>27.281</v>
+      </c>
+      <c r="AX6" s="2" t="inlineStr"/>
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" t="n">
+        <v>1.220230579376221</v>
+      </c>
+      <c r="B7" t="n">
+        <v>3.601427555084229</v>
+      </c>
+      <c r="C7" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>6</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1.192</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-10.7707</v>
+      </c>
+      <c r="H7" t="n">
+        <v>6.005444</v>
+      </c>
+      <c r="I7" t="n">
+        <v>5.838497162</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-43.88553238</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.1202778816223145</v>
+      </c>
+      <c r="L7" t="n">
+        <v>5.91196155548</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-51.5794992447</v>
+      </c>
+      <c r="N7" t="n">
+        <v>-52.9670495987</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.1932497024536133</v>
+      </c>
+      <c r="P7" t="n">
+        <v>5.791469574</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-50.85944366</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.1074469089508057</v>
+      </c>
+      <c r="S7" t="n">
+        <v>5.89789676666</v>
+      </c>
+      <c r="T7" t="n">
+        <v>-50.125210762</v>
+      </c>
+      <c r="U7" t="n">
+        <v>-52.4777765274</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0.1501402854919434</v>
+      </c>
+      <c r="W7" t="n">
+        <v>6.274209260940552</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0.186</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>5.887290955</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>-49.04273224</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>0.1730093955993652</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>6.00402545929</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>-48.8432817459</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>-50.3793001175</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>0.1541531085968018</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>2.798098087310791</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>0.436</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>5.92755127</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>-49.1100502</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>0.1650357246398926</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>6.00565910339</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>-59.1627941132</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>-59.5720386505</v>
+      </c>
+      <c r="AR7" t="n">
+        <v>0.1917657852172852</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>9.409790992736816</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>0.432</v>
+      </c>
+      <c r="AW7" t="n">
+        <v>26.005</v>
+      </c>
+      <c r="AX7" s="2" t="inlineStr"/>
+    </row>
+    <row r="8" ht="15" customHeight="1">
+      <c r="A8" t="n">
+        <v>1.220230579376221</v>
+      </c>
+      <c r="B8" t="n">
+        <v>3.601427555084229</v>
+      </c>
+      <c r="C8" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="D8" t="n">
+        <v>6</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.191</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-10.74574</v>
+      </c>
+      <c r="H8" t="n">
+        <v>6.011664</v>
+      </c>
+      <c r="I8" t="n">
+        <v>5.96836853</v>
+      </c>
+      <c r="J8" t="n">
+        <v>-43.80942535</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.07971286773681641</v>
+      </c>
+      <c r="L8" t="n">
+        <v>6.04242086411</v>
+      </c>
+      <c r="M8" t="n">
+        <v>-51.6768660545</v>
+      </c>
+      <c r="N8" t="n">
+        <v>-53.306283474</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.1866886615753174</v>
+      </c>
+      <c r="P8" t="n">
+        <v>5.921043396</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>-50.95992661</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.08726811408996582</v>
+      </c>
+      <c r="S8" t="n">
+        <v>6.03580713272</v>
+      </c>
+      <c r="T8" t="n">
+        <v>-49.1943421364</v>
+      </c>
+      <c r="U8" t="n">
+        <v>-52.8759865761</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.1773674488067627</v>
+      </c>
+      <c r="W8" t="n">
+        <v>6.246154546737671</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>5.918746948</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>-48.86702728</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>0.2074992656707764</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>6.03691387177</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>-47.9476156235</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>-50.5188627243</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>0.1777260303497314</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>2.776440382003784</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>0.413</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>5.953157425</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>-49.09585953</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>0.1705596446990967</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>6.03079891205</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>-59.3464918137</v>
+      </c>
+      <c r="AQ8" t="n">
+        <v>-59.8654317856</v>
+      </c>
+      <c r="AR8" t="n">
+        <v>0.1938447952270508</v>
+      </c>
+      <c r="AS8" t="n">
+        <v>9.272533416748047</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV8" t="n">
+        <v>0.399</v>
+      </c>
+      <c r="AW8" t="n">
+        <v>26.135</v>
+      </c>
+      <c r="AX8" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1053,7 +1789,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -1063,7 +1799,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4.544441938400269</v>
+        <v>1.220230579376221</v>
       </c>
     </row>
     <row r="4">
@@ -1073,7 +1809,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4.544441938400269</v>
+        <v>1.220230579376221</v>
       </c>
     </row>
     <row r="5">
@@ -1083,7 +1819,7 @@
         </is>
       </c>
       <c r="B5" s="4" t="n">
-        <v>4.544441938400269</v>
+        <v>1.220230579376221</v>
       </c>
     </row>
     <row r="6">
@@ -1093,7 +1829,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>13.52477216720581</v>
+        <v>3.601427555084229</v>
       </c>
     </row>
     <row r="7">
@@ -1103,7 +1839,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>13.52477216720581</v>
+        <v>3.601427555084229</v>
       </c>
     </row>
     <row r="8">
@@ -1113,7 +1849,7 @@
         </is>
       </c>
       <c r="B8" s="4" t="n">
-        <v>13.52477216720581</v>
+        <v>3.601427555084229</v>
       </c>
     </row>
     <row r="9">
@@ -1123,7 +1859,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2.1</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="10">
@@ -1133,7 +1869,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
@@ -1143,7 +1879,7 @@
         </is>
       </c>
       <c r="B11" s="4" t="n">
-        <v>2.05</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="12">
@@ -1153,7 +1889,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
@@ -1163,7 +1899,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14">
@@ -1173,7 +1909,7 @@
         </is>
       </c>
       <c r="B14" s="4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15">
@@ -1183,7 +1919,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -1203,7 +1939,7 @@
         </is>
       </c>
       <c r="B17" s="4" t="n">
-        <v>1</v>
+        <v>1.428571428571429</v>
       </c>
     </row>
     <row r="18">
@@ -1213,7 +1949,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.393</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="19">
@@ -1223,7 +1959,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.352</v>
+        <v>0.403</v>
       </c>
     </row>
     <row r="20">
@@ -1233,7 +1969,7 @@
         </is>
       </c>
       <c r="B20" s="4" t="n">
-        <v>0.3725</v>
+        <v>0.8201428571428571</v>
       </c>
     </row>
     <row r="21">
@@ -1243,7 +1979,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-13.43059</v>
+        <v>-10.71387</v>
       </c>
     </row>
     <row r="22">
@@ -1253,7 +1989,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-13.47612</v>
+        <v>-10.99513</v>
       </c>
     </row>
     <row r="23">
@@ -1263,7 +1999,7 @@
         </is>
       </c>
       <c r="B23" s="4" t="n">
-        <v>-13.453355</v>
+        <v>-10.85039</v>
       </c>
     </row>
     <row r="24">
@@ -1273,7 +2009,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>5.085418</v>
+        <v>6.032585</v>
       </c>
     </row>
     <row r="25">
@@ -1283,7 +2019,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>5.036761</v>
+        <v>5.929387</v>
       </c>
     </row>
     <row r="26">
@@ -1293,7 +2029,7 @@
         </is>
       </c>
       <c r="B26" s="4" t="n">
-        <v>5.0610895</v>
+        <v>5.98934</v>
       </c>
     </row>
     <row r="27">
@@ -1303,7 +2039,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>4.976383209</v>
+        <v>5.96836853</v>
       </c>
     </row>
     <row r="28">
@@ -1313,7 +2049,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>4.908203125</v>
+        <v>5.838497162</v>
       </c>
     </row>
     <row r="29">
@@ -1323,7 +2059,7 @@
         </is>
       </c>
       <c r="B29" s="4" t="n">
-        <v>4.942293167</v>
+        <v>5.921700341285714</v>
       </c>
     </row>
     <row r="30">
@@ -1333,7 +2069,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-21.40676689</v>
+        <v>-43.79166031</v>
       </c>
     </row>
     <row r="31">
@@ -1343,7 +2079,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-47.23838425</v>
+        <v>-44.29456329</v>
       </c>
     </row>
     <row r="32">
@@ -1353,7 +2089,7 @@
         </is>
       </c>
       <c r="B32" s="4" t="n">
-        <v>-34.32257557</v>
+        <v>-43.95294080285714</v>
       </c>
     </row>
     <row r="33">
@@ -1363,7 +2099,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.1952049732208252</v>
+        <v>0.1474802494049072</v>
       </c>
     </row>
     <row r="34">
@@ -1373,7 +2109,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.1922016143798828</v>
+        <v>0.07971286773681641</v>
       </c>
     </row>
     <row r="35">
@@ -1383,7 +2119,7 @@
         </is>
       </c>
       <c r="B35" s="4" t="n">
-        <v>0.193703293800354</v>
+        <v>0.1047137805393764</v>
       </c>
     </row>
     <row r="36">
@@ -1393,7 +2129,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>5.02750635147</v>
+        <v>6.04576396942</v>
       </c>
     </row>
     <row r="37">
@@ -1403,7 +2139,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>4.97490406036</v>
+        <v>5.91196155548</v>
       </c>
     </row>
     <row r="38">
@@ -1413,7 +2149,7 @@
         </is>
       </c>
       <c r="B38" s="4" t="n">
-        <v>5.001205205914999</v>
+        <v>5.988005297524285</v>
       </c>
     </row>
     <row r="39">
@@ -1423,7 +2159,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>-55.1714296341</v>
+        <v>-51.4035868645</v>
       </c>
     </row>
     <row r="40">
@@ -1433,7 +2169,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>-55.1757493019</v>
+        <v>-52.0992126465</v>
       </c>
     </row>
     <row r="41">
@@ -1443,7 +2179,7 @@
         </is>
       </c>
       <c r="B41" s="4" t="n">
-        <v>-55.173589468</v>
+        <v>-51.7385638782</v>
       </c>
     </row>
     <row r="42">
@@ -1453,7 +2189,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>-56.3040742874</v>
+        <v>-52.8622965813</v>
       </c>
     </row>
     <row r="43">
@@ -1463,7 +2199,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>-56.4646325111</v>
+        <v>-53.5028305054</v>
       </c>
     </row>
     <row r="44">
@@ -1473,7 +2209,7 @@
         </is>
       </c>
       <c r="B44" s="4" t="n">
-        <v>-56.38435339925</v>
+        <v>-53.19225072862857</v>
       </c>
     </row>
     <row r="45">
@@ -1483,7 +2219,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.217111349105835</v>
+        <v>0.1998167037963867</v>
       </c>
     </row>
     <row r="46">
@@ -1493,7 +2229,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.1937520503997803</v>
+        <v>0.186129093170166</v>
       </c>
     </row>
     <row r="47">
@@ -1503,7 +2239,7 @@
         </is>
       </c>
       <c r="B47" s="4" t="n">
-        <v>0.2054316997528076</v>
+        <v>0.1926859446934291</v>
       </c>
     </row>
     <row r="48">
@@ -1513,7 +2249,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>5.057008743</v>
+        <v>5.971302032</v>
       </c>
     </row>
     <row r="49">
@@ -1523,7 +2259,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>4.908157349</v>
+        <v>5.791469574</v>
       </c>
     </row>
     <row r="50">
@@ -1533,7 +2269,7 @@
         </is>
       </c>
       <c r="B50" s="4" t="n">
-        <v>4.982583046</v>
+        <v>5.896333422</v>
       </c>
     </row>
     <row r="51">
@@ -1543,7 +2279,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>-21.40340424</v>
+        <v>-50.41112518</v>
       </c>
     </row>
     <row r="52">
@@ -1553,7 +2289,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>-50.3416481</v>
+        <v>-50.95992661</v>
       </c>
     </row>
     <row r="53">
@@ -1563,7 +2299,7 @@
         </is>
       </c>
       <c r="B53" s="4" t="n">
-        <v>-35.87252617</v>
+        <v>-50.71074894571429</v>
       </c>
     </row>
     <row r="54">
@@ -1573,7 +2309,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.2275807857513428</v>
+        <v>0.1074469089508057</v>
       </c>
     </row>
     <row r="55">
@@ -1583,7 +2319,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.1980037689208984</v>
+        <v>0.04189252853393555</v>
       </c>
     </row>
     <row r="56">
@@ -1593,7 +2329,7 @@
         </is>
       </c>
       <c r="B56" s="4" t="n">
-        <v>0.2127922773361206</v>
+        <v>0.08371394021170479</v>
       </c>
     </row>
     <row r="57">
@@ -1603,7 +2339,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>5.10628175735</v>
+        <v>6.05037403107</v>
       </c>
     </row>
     <row r="58">
@@ -1613,7 +2349,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>4.98175525665</v>
+        <v>5.89789676666</v>
       </c>
     </row>
     <row r="59">
@@ -1623,7 +2359,7 @@
         </is>
       </c>
       <c r="B59" s="4" t="n">
-        <v>5.044018507</v>
+        <v>6.004754815782857</v>
       </c>
     </row>
     <row r="60">
@@ -1633,7 +2369,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>-55.0589227676</v>
+        <v>-49.1943421364</v>
       </c>
     </row>
     <row r="61">
@@ -1643,7 +2379,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>-60.6061177254</v>
+        <v>-50.4292626381</v>
       </c>
     </row>
     <row r="62">
@@ -1653,7 +2389,7 @@
         </is>
       </c>
       <c r="B62" s="4" t="n">
-        <v>-57.8325202465</v>
+        <v>-49.69081013542858</v>
       </c>
     </row>
     <row r="63">
@@ -1663,7 +2399,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>-56.2393503189</v>
+        <v>-52.0804390907</v>
       </c>
     </row>
     <row r="64">
@@ -1673,7 +2409,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>-60.3064007759</v>
+        <v>-52.8759865761</v>
       </c>
     </row>
     <row r="65">
@@ -1683,7 +2419,7 @@
         </is>
       </c>
       <c r="B65" s="4" t="n">
-        <v>-58.27287554740001</v>
+        <v>-52.45847054888571</v>
       </c>
     </row>
     <row r="66">
@@ -1693,7 +2429,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.1907782554626465</v>
+        <v>0.1858205795288086</v>
       </c>
     </row>
     <row r="67">
@@ -1703,7 +2439,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.185863733291626</v>
+        <v>0.1501402854919434</v>
       </c>
     </row>
     <row r="68">
@@ -1713,7 +2449,7 @@
         </is>
       </c>
       <c r="B68" s="4" t="n">
-        <v>0.1883209943771362</v>
+        <v>0.1724098069327218</v>
       </c>
     </row>
     <row r="69">
@@ -1723,7 +2459,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>6.935030698776245</v>
+        <v>7.333505630493164</v>
       </c>
     </row>
     <row r="70">
@@ -1733,7 +2469,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>3.048375129699707</v>
+        <v>6.246154546737671</v>
       </c>
     </row>
     <row r="71">
@@ -1743,7 +2479,7 @@
         </is>
       </c>
       <c r="B71" s="4" t="n">
-        <v>4.991702914237976</v>
+        <v>6.778385741370065</v>
       </c>
     </row>
     <row r="72">
@@ -1813,7 +2549,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>2.638</v>
+        <v>0.409</v>
       </c>
     </row>
     <row r="79">
@@ -1823,7 +2559,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>1.218</v>
+        <v>0.176</v>
       </c>
     </row>
     <row r="80">
@@ -1833,7 +2569,7 @@
         </is>
       </c>
       <c r="B80" s="4" t="n">
-        <v>1.928</v>
+        <v>0.2192857142857143</v>
       </c>
     </row>
     <row r="81">
@@ -1843,7 +2579,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>5.009925842</v>
+        <v>5.985588074</v>
       </c>
     </row>
     <row r="82">
@@ -1853,7 +2589,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>4.986499786</v>
+        <v>5.887290955</v>
       </c>
     </row>
     <row r="83">
@@ -1863,7 +2599,7 @@
         </is>
       </c>
       <c r="B83" s="4" t="n">
-        <v>4.998212814</v>
+        <v>5.940581458</v>
       </c>
     </row>
     <row r="84">
@@ -1873,7 +2609,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>-49.20523834</v>
+        <v>-48.86702728</v>
       </c>
     </row>
     <row r="85">
@@ -1883,7 +2619,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>-50.09896851</v>
+        <v>-49.75502396</v>
       </c>
     </row>
     <row r="86">
@@ -1893,7 +2629,7 @@
         </is>
       </c>
       <c r="B86" s="4" t="n">
-        <v>-49.652103425</v>
+        <v>-49.16301672714285</v>
       </c>
     </row>
     <row r="87">
@@ -1903,7 +2639,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0.3543787002563477</v>
+        <v>0.2074992656707764</v>
       </c>
     </row>
     <row r="88">
@@ -1913,7 +2649,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>0.3401844501495361</v>
+        <v>0.1377959251403809</v>
       </c>
     </row>
     <row r="89">
@@ -1923,7 +2659,7 @@
         </is>
       </c>
       <c r="B89" s="4" t="n">
-        <v>0.3472815752029419</v>
+        <v>0.1742212431771415</v>
       </c>
     </row>
     <row r="90">
@@ -1933,7 +2669,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>5.07956218719</v>
+        <v>6.11211681366</v>
       </c>
     </row>
     <row r="91">
@@ -1943,7 +2679,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>5.03555059433</v>
+        <v>6.00402545929</v>
       </c>
     </row>
     <row r="92">
@@ -1953,7 +2689,7 @@
         </is>
       </c>
       <c r="B92" s="4" t="n">
-        <v>5.05755639076</v>
+        <v>6.051643644060001</v>
       </c>
     </row>
     <row r="93">
@@ -1963,7 +2699,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>-54.4045591354</v>
+        <v>-47.9476156235</v>
       </c>
     </row>
     <row r="94">
@@ -1973,7 +2709,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>-55.7622961998</v>
+        <v>-48.8432817459</v>
       </c>
     </row>
     <row r="95">
@@ -1983,7 +2719,7 @@
         </is>
       </c>
       <c r="B95" s="4" t="n">
-        <v>-55.0834276676</v>
+        <v>-48.53581210545714</v>
       </c>
     </row>
     <row r="96">
@@ -1993,7 +2729,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>-55.4119215012</v>
+        <v>-50.1791052818</v>
       </c>
     </row>
     <row r="97">
@@ -2003,7 +2739,7 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>-55.8825850487</v>
+        <v>-50.8653478622</v>
       </c>
     </row>
     <row r="98">
@@ -2013,7 +2749,7 @@
         </is>
       </c>
       <c r="B98" s="4" t="n">
-        <v>-55.64725327495</v>
+        <v>-50.45172582352857</v>
       </c>
     </row>
     <row r="99">
@@ -2023,7 +2759,7 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>0.186917781829834</v>
+        <v>0.1806857585906982</v>
       </c>
     </row>
     <row r="100">
@@ -2033,7 +2769,7 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>0.1863663196563721</v>
+        <v>0.1530272960662842</v>
       </c>
     </row>
     <row r="101">
@@ -2043,7 +2779,7 @@
         </is>
       </c>
       <c r="B101" s="4" t="n">
-        <v>0.186642050743103</v>
+        <v>0.1706716333116804</v>
       </c>
     </row>
     <row r="102">
@@ -2053,7 +2789,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>11.80976676940918</v>
+        <v>2.836046457290649</v>
       </c>
     </row>
     <row r="103">
@@ -2063,7 +2799,7 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>11.75644135475159</v>
+        <v>2.707039833068848</v>
       </c>
     </row>
     <row r="104">
@@ -2073,7 +2809,7 @@
         </is>
       </c>
       <c r="B104" s="4" t="n">
-        <v>11.78310406208038</v>
+        <v>2.766511610576085</v>
       </c>
     </row>
     <row r="105">
@@ -2143,7 +2879,7 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>2.571</v>
+        <v>0.436</v>
       </c>
     </row>
     <row r="112">
@@ -2153,7 +2889,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>2.545</v>
+        <v>0.384</v>
       </c>
     </row>
     <row r="113">
@@ -2163,7 +2899,7 @@
         </is>
       </c>
       <c r="B113" s="4" t="n">
-        <v>2.558</v>
+        <v>0.4114285714285714</v>
       </c>
     </row>
     <row r="114">
@@ -2173,7 +2909,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>5.010688782</v>
+        <v>5.953754425</v>
       </c>
     </row>
     <row r="115">
@@ -2183,7 +2919,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>4.984535217</v>
+        <v>5.913640976</v>
       </c>
     </row>
     <row r="116">
@@ -2193,7 +2929,7 @@
         </is>
       </c>
       <c r="B116" s="4" t="n">
-        <v>4.9976119995</v>
+        <v>5.933791024428571</v>
       </c>
     </row>
     <row r="117">
@@ -2203,7 +2939,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>-49.71195221</v>
+        <v>-49.09585953</v>
       </c>
     </row>
     <row r="118">
@@ -2213,7 +2949,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>-50.68193817</v>
+        <v>-50.27392578</v>
       </c>
     </row>
     <row r="119">
@@ -2223,7 +2959,7 @@
         </is>
       </c>
       <c r="B119" s="4" t="n">
-        <v>-50.19694519</v>
+        <v>-49.57655552428571</v>
       </c>
     </row>
     <row r="120">
@@ -2233,7 +2969,7 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>0.3320817947387695</v>
+        <v>0.1705596446990967</v>
       </c>
     </row>
     <row r="121">
@@ -2243,7 +2979,7 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>0.3266315460205078</v>
+        <v>0.1237905025482178</v>
       </c>
     </row>
     <row r="122">
@@ -2253,7 +2989,7 @@
         </is>
       </c>
       <c r="B122" s="4" t="n">
-        <v>0.3293566703796387</v>
+        <v>0.1512487956455776</v>
       </c>
     </row>
     <row r="123">
@@ -2263,7 +2999,7 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>5.0837225914</v>
+        <v>6.04695129395</v>
       </c>
     </row>
     <row r="124">
@@ -2273,7 +3009,7 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>5.04499912262</v>
+        <v>5.94747495651</v>
       </c>
     </row>
     <row r="125">
@@ -2283,7 +3019,7 @@
         </is>
       </c>
       <c r="B125" s="4" t="n">
-        <v>5.06436085701</v>
+        <v>6.004153319767143</v>
       </c>
     </row>
     <row r="126">
@@ -2293,7 +3029,7 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>-58.7719774246</v>
+        <v>-59.1627941132</v>
       </c>
     </row>
     <row r="127">
@@ -2303,7 +3039,7 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>-60.4407744408</v>
+        <v>-60.7487335205</v>
       </c>
     </row>
     <row r="128">
@@ -2313,7 +3049,7 @@
         </is>
       </c>
       <c r="B128" s="4" t="n">
-        <v>-59.6063759327</v>
+        <v>-59.95392847062858</v>
       </c>
     </row>
     <row r="129">
@@ -2323,7 +3059,7 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>-58.9627084732</v>
+        <v>-59.5720386505</v>
       </c>
     </row>
     <row r="130">
@@ -2333,7 +3069,7 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>-60.4873366356</v>
+        <v>-61.0186157227</v>
       </c>
     </row>
     <row r="131">
@@ -2343,7 +3079,7 @@
         </is>
       </c>
       <c r="B131" s="4" t="n">
-        <v>-59.7250225544</v>
+        <v>-60.23249074391428</v>
       </c>
     </row>
     <row r="132">
@@ -2353,7 +3089,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>0.1902198791503906</v>
+        <v>0.1987082958221436</v>
       </c>
     </row>
     <row r="133">
@@ -2363,7 +3099,7 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>0.1884052753448486</v>
+        <v>0.1886463165283203</v>
       </c>
     </row>
     <row r="134">
@@ -2373,7 +3109,7 @@
         </is>
       </c>
       <c r="B134" s="4" t="n">
-        <v>0.1893125772476196</v>
+        <v>0.192969696862357</v>
       </c>
     </row>
     <row r="135">
@@ -2383,7 +3119,7 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>21.41870021820068</v>
+        <v>9.742092847824097</v>
       </c>
     </row>
     <row r="136">
@@ -2393,7 +3129,7 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>20.66013479232788</v>
+        <v>9.272533416748047</v>
       </c>
     </row>
     <row r="137">
@@ -2403,7 +3139,7 @@
         </is>
       </c>
       <c r="B137" s="4" t="n">
-        <v>21.03941750526428</v>
+        <v>9.401362827845983</v>
       </c>
     </row>
     <row r="138">
@@ -2473,7 +3209,7 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>2.594</v>
+        <v>0.446</v>
       </c>
     </row>
     <row r="145">
@@ -2483,7 +3219,7 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>2.566</v>
+        <v>0.399</v>
       </c>
     </row>
     <row r="146">
@@ -2493,7 +3229,7 @@
         </is>
       </c>
       <c r="B146" s="4" t="n">
-        <v>2.58</v>
+        <v>0.4248571428571429</v>
       </c>
     </row>
     <row r="147">
@@ -2503,7 +3239,7 @@
         </is>
       </c>
       <c r="B147" t="n">
-        <v>41.271</v>
+        <v>27.307</v>
       </c>
     </row>
     <row r="148">
@@ -2513,7 +3249,7 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>36.657</v>
+        <v>26.005</v>
       </c>
     </row>
     <row r="149">
@@ -2523,7 +3259,7 @@
         </is>
       </c>
       <c r="B149" s="4" t="n">
-        <v>38.964</v>
+        <v>26.75242857142857</v>
       </c>
     </row>
   </sheetData>

</xml_diff>